<commit_message>
coluna de ultima atualizacao
</commit_message>
<xml_diff>
--- a/arquivo_formatado.xlsx
+++ b/arquivo_formatado.xlsx
@@ -1068,7 +1068,7 @@
     <row r="18" ht="142.5" customHeight="1">
       <c r="A18" s="7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Na montagem das laterais foi observado um erro no componente: 240642 - GANCHO MENOR P/ F.RÁPIDO CÓD.FT 0040-C - Saldo: 300,00 - Consumo Médio Mensal: 87,67. Onde foram inspecionando os 100,00 na produção mais os 300,00 no almoxarifado. Do total dos 400,00 foi encontrado 47,00 unidades com não conformidades que não podem ser aproveitadas. </t>
+          <t>https://cemag.monday.com/protected_static/12861583/resources/947643825/ev%202.jpg, https://cemag.monday.com/protected_static/12861583/resources/947643833/ev%201.jpg</t>
         </is>
       </c>
       <c r="B18" s="41" t="n"/>
@@ -1092,7 +1092,7 @@
     <row r="20" ht="19.5" customHeight="1">
       <c r="A20" s="7" t="inlineStr">
         <is>
-          <t>https://cemag.monday.com/protected_static/12861583/resources/947643825/ev%202.jpg, https://cemag.monday.com/protected_static/12861583/resources/947643833/ev%201.jpg</t>
+          <t xml:space="preserve">Na montagem das laterais foi observado um erro no componente: 240642 - GANCHO MENOR P/ F.RÁPIDO CÓD.FT 0040-C - Saldo: 300,00 - Consumo Médio Mensal: 87,67. Onde foram inspecionando os 100,00 na produção mais os 300,00 no almoxarifado. Do total dos 400,00 foi encontrado 47,00 unidades com não conformidades que não podem ser aproveitadas. </t>
         </is>
       </c>
       <c r="B20" s="41" t="n"/>
@@ -1157,79 +1157,33 @@
         </is>
       </c>
       <c r="C23" s="8" t="inlineStr"/>
-      <c r="D23" s="9" t="inlineStr">
-        <is>
-          <t>Estefane Santos, Severiano Neto</t>
-        </is>
-      </c>
-      <c r="E23" s="9" t="inlineStr">
-        <is>
-          <t>Feito</t>
-        </is>
-      </c>
-      <c r="F23" s="9" t="n">
-        <v>5</v>
-      </c>
+      <c r="D23" s="9" t="n"/>
+      <c r="E23" s="9" t="n"/>
+      <c r="F23" s="9" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="6" t="inlineStr">
-        <is>
-          <t>Almoxarifado</t>
-        </is>
-      </c>
-      <c r="B24" s="7" t="inlineStr">
-        <is>
-          <t>Tranferir 47 peças do componente:240642 - GANCHO MENOR P/ F.RÁPIDO CÓD.FT 0040-C  para o estoque da qualidade</t>
-        </is>
-      </c>
-      <c r="C24" s="8" t="inlineStr"/>
-      <c r="D24" s="9" t="inlineStr">
-        <is>
-          <t>victor@cemag.com.br</t>
-        </is>
-      </c>
-      <c r="E24" s="9" t="inlineStr">
-        <is>
-          <t>Feito</t>
-        </is>
-      </c>
-      <c r="F24" s="9" t="n">
-        <v>5</v>
-      </c>
+      <c r="A24" s="6" t="n"/>
+      <c r="B24" s="7" t="n"/>
+      <c r="C24" s="8" t="n"/>
+      <c r="D24" s="9" t="n"/>
+      <c r="E24" s="9" t="n"/>
+      <c r="F24" s="9" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="6" t="inlineStr">
-        <is>
-          <t>Compras</t>
-        </is>
-      </c>
-      <c r="B25" s="7" t="inlineStr">
-        <is>
-          <t>Entrar em contato com fornecedor do componente: 240642 - GANCHO MENOR P/ F.RÁPIDO CÓD.FT 0040-C , para informar sobre as 47 unidades de peças nao conformes encontradas.</t>
-        </is>
-      </c>
-      <c r="C25" s="8" t="inlineStr"/>
-      <c r="D25" s="9" t="inlineStr">
-        <is>
-          <t>lauriene@cemag.com.br</t>
-        </is>
-      </c>
-      <c r="E25" s="9" t="inlineStr">
-        <is>
-          <t>Feito</t>
-        </is>
-      </c>
-      <c r="F25" s="9" t="n">
-        <v>5</v>
-      </c>
+      <c r="A25" s="6" t="n"/>
+      <c r="B25" s="7" t="n"/>
+      <c r="C25" s="8" t="n"/>
+      <c r="D25" s="9" t="n"/>
+      <c r="E25" s="9" t="n"/>
+      <c r="F25" s="9" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="6" t="inlineStr"/>
-      <c r="B26" s="7" t="inlineStr"/>
-      <c r="C26" s="8" t="inlineStr"/>
-      <c r="D26" s="9" t="inlineStr"/>
-      <c r="E26" s="9" t="inlineStr"/>
-      <c r="F26" s="9" t="inlineStr"/>
+      <c r="A26" s="6" t="n"/>
+      <c r="B26" s="7" t="n"/>
+      <c r="C26" s="8" t="n"/>
+      <c r="D26" s="9" t="n"/>
+      <c r="E26" s="9" t="n"/>
+      <c r="F26" s="9" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="6" t="n"/>

</xml_diff>

<commit_message>
versao final com mudanças solicitadas pela Estefane dia 06/12/2023
</commit_message>
<xml_diff>
--- a/arquivo_formatado.xlsx
+++ b/arquivo_formatado.xlsx
@@ -598,186 +598,63 @@
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color rgb="FFC6C6C6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFC6C6C6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFC6C6C6"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFC6C6C6"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FFC6C6C6"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFC6C6C6"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFC6C6C6"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFC6C6C6"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFC6C6C6"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFC6C6C6"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFC6C6C6"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFC6C6C6"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -801,17 +678,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -824,6 +690,17 @@
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top/>
       <bottom style="thin">
@@ -834,19 +711,142 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFC6C6C6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFC6C6C6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFC6C6C6"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFC6C6C6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC6C6C6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFC6C6C6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC6C6C6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFC6C6C6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFC6C6C6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC6C6C6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFC6C6C6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC6C6C6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFC6C6C6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC6C6C6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC6C6C6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFC6C6C6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
@@ -914,263 +914,254 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="21" fontId="7" fillId="0" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="5" borderId="35" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="5" borderId="36" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="3" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="33" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="37" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="38" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="33" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="37" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="5" borderId="35" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="5" borderId="36" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="3" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="38" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="21" fontId="7" fillId="0" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -1192,43 +1183,43 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="52" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="54" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="60" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="14" fontId="10" fillId="5" borderId="51" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="14" fontId="10" fillId="5" borderId="41" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -1637,42 +1628,42 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA46"/>
+  <dimension ref="A1:AA51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20.28515625" bestFit="1" customWidth="1" style="57" min="1" max="1"/>
-    <col width="19.5703125" bestFit="1" customWidth="1" style="57" min="2" max="2"/>
-    <col width="17.5703125" bestFit="1" customWidth="1" style="57" min="3" max="4"/>
-    <col width="28.85546875" bestFit="1" customWidth="1" style="57" min="5" max="5"/>
-    <col width="12.85546875" bestFit="1" customWidth="1" style="57" min="6" max="6"/>
-    <col width="17.140625" bestFit="1" customWidth="1" style="57" min="7" max="7"/>
-    <col width="18.28515625" customWidth="1" style="57" min="8" max="8"/>
-    <col width="28.28515625" customWidth="1" style="58" min="9" max="9"/>
+    <col width="20.28515625" bestFit="1" customWidth="1" style="25" min="1" max="1"/>
+    <col width="19.5703125" bestFit="1" customWidth="1" style="25" min="2" max="2"/>
+    <col width="17.5703125" bestFit="1" customWidth="1" style="25" min="3" max="4"/>
+    <col width="28.85546875" bestFit="1" customWidth="1" style="25" min="5" max="5"/>
+    <col width="12.85546875" bestFit="1" customWidth="1" style="25" min="6" max="6"/>
+    <col width="17.140625" bestFit="1" customWidth="1" style="25" min="7" max="7"/>
+    <col width="18.28515625" customWidth="1" style="25" min="8" max="8"/>
+    <col width="28.28515625" customWidth="1" style="26" min="9" max="9"/>
     <col width="13.5703125" bestFit="1" customWidth="1" min="10" max="27"/>
   </cols>
   <sheetData>
     <row r="1" ht="23.25" customHeight="1">
-      <c r="A1" s="109" t="n"/>
-      <c r="B1" s="110" t="inlineStr">
+      <c r="A1" s="106" t="n"/>
+      <c r="B1" s="107" t="inlineStr">
         <is>
           <t>Relatório de Não Conformidade</t>
         </is>
       </c>
-      <c r="C1" s="111" t="n"/>
-      <c r="D1" s="111" t="n"/>
-      <c r="E1" s="111" t="n"/>
-      <c r="F1" s="112" t="n"/>
-      <c r="G1" s="113" t="inlineStr">
+      <c r="C1" s="108" t="n"/>
+      <c r="D1" s="108" t="n"/>
+      <c r="E1" s="108" t="n"/>
+      <c r="F1" s="109" t="n"/>
+      <c r="G1" s="110" t="inlineStr">
         <is>
           <t>Código:</t>
         </is>
       </c>
-      <c r="H1" s="114" t="n"/>
+      <c r="H1" s="111" t="n"/>
       <c r="I1" s="3" t="inlineStr">
         <is>
           <t>RNC GQ-001-000</t>
@@ -1680,91 +1671,91 @@
       </c>
     </row>
     <row r="2" ht="23.25" customHeight="1">
-      <c r="A2" s="115" t="n"/>
-      <c r="B2" s="116" t="n"/>
-      <c r="C2" s="117" t="n"/>
-      <c r="D2" s="117" t="n"/>
-      <c r="E2" s="117" t="n"/>
-      <c r="F2" s="118" t="n"/>
-      <c r="G2" s="113" t="inlineStr">
+      <c r="A2" s="112" t="n"/>
+      <c r="B2" s="113" t="n"/>
+      <c r="C2" s="114" t="n"/>
+      <c r="D2" s="114" t="n"/>
+      <c r="E2" s="114" t="n"/>
+      <c r="F2" s="115" t="n"/>
+      <c r="G2" s="110" t="inlineStr">
         <is>
           <t>Data de Emissão:</t>
         </is>
       </c>
-      <c r="H2" s="114" t="n"/>
+      <c r="H2" s="111" t="n"/>
       <c r="I2" s="4" t="n">
         <v>44487</v>
       </c>
     </row>
     <row r="3" ht="23.25" customHeight="1">
-      <c r="A3" s="115" t="n"/>
-      <c r="B3" s="119" t="inlineStr">
+      <c r="A3" s="112" t="n"/>
+      <c r="B3" s="116" t="inlineStr">
         <is>
           <t>Gestão da Qualidade</t>
         </is>
       </c>
-      <c r="C3" s="111" t="n"/>
-      <c r="D3" s="111" t="n"/>
-      <c r="E3" s="111" t="n"/>
-      <c r="F3" s="112" t="n"/>
-      <c r="G3" s="113" t="inlineStr">
+      <c r="C3" s="108" t="n"/>
+      <c r="D3" s="108" t="n"/>
+      <c r="E3" s="108" t="n"/>
+      <c r="F3" s="109" t="n"/>
+      <c r="G3" s="110" t="inlineStr">
         <is>
           <t>Data da Última Revisão:</t>
         </is>
       </c>
-      <c r="H3" s="114" t="n"/>
+      <c r="H3" s="111" t="n"/>
       <c r="I3" s="5" t="n"/>
     </row>
     <row r="4" ht="24" customHeight="1">
-      <c r="A4" s="120" t="n"/>
-      <c r="B4" s="116" t="n"/>
-      <c r="C4" s="117" t="n"/>
-      <c r="D4" s="117" t="n"/>
-      <c r="E4" s="117" t="n"/>
-      <c r="F4" s="118" t="n"/>
-      <c r="G4" s="113" t="inlineStr">
+      <c r="A4" s="117" t="n"/>
+      <c r="B4" s="113" t="n"/>
+      <c r="C4" s="114" t="n"/>
+      <c r="D4" s="114" t="n"/>
+      <c r="E4" s="114" t="n"/>
+      <c r="F4" s="115" t="n"/>
+      <c r="G4" s="110" t="inlineStr">
         <is>
           <t>Página:</t>
         </is>
       </c>
-      <c r="H4" s="114" t="n"/>
+      <c r="H4" s="111" t="n"/>
       <c r="I4" s="6" t="n">
         <v>44197</v>
       </c>
     </row>
     <row r="5" ht="18.75" customHeight="1">
-      <c r="A5" s="35" t="n"/>
-      <c r="B5" s="111" t="n"/>
-      <c r="C5" s="111" t="n"/>
-      <c r="D5" s="111" t="n"/>
-      <c r="E5" s="111" t="n"/>
-      <c r="F5" s="111" t="n"/>
-      <c r="G5" s="111" t="n"/>
-      <c r="H5" s="111" t="n"/>
-      <c r="I5" s="111" t="n"/>
+      <c r="A5" s="94" t="n"/>
+      <c r="B5" s="108" t="n"/>
+      <c r="C5" s="108" t="n"/>
+      <c r="D5" s="108" t="n"/>
+      <c r="E5" s="108" t="n"/>
+      <c r="F5" s="108" t="n"/>
+      <c r="G5" s="108" t="n"/>
+      <c r="H5" s="108" t="n"/>
+      <c r="I5" s="108" t="n"/>
     </row>
     <row r="6" ht="24.75" customHeight="1">
-      <c r="A6" s="37" t="inlineStr">
+      <c r="A6" s="96" t="inlineStr">
         <is>
           <t>1ª ETAPA - ABERTURA</t>
         </is>
       </c>
-      <c r="B6" s="111" t="n"/>
-      <c r="C6" s="111" t="n"/>
-      <c r="D6" s="111" t="n"/>
-      <c r="E6" s="121" t="n"/>
+      <c r="B6" s="108" t="n"/>
+      <c r="C6" s="108" t="n"/>
+      <c r="D6" s="108" t="n"/>
+      <c r="E6" s="118" t="n"/>
       <c r="F6" s="7" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="G6" s="38" t="inlineStr">
+      <c r="G6" s="97" t="inlineStr">
         <is>
           <t>Feito</t>
         </is>
       </c>
-      <c r="H6" s="122" t="n"/>
-      <c r="I6" s="123" t="n"/>
+      <c r="H6" s="119" t="n"/>
+      <c r="I6" s="120" t="n"/>
       <c r="J6" s="1" t="n"/>
       <c r="K6" s="1" t="n"/>
       <c r="L6" s="2" t="n"/>
@@ -1785,123 +1776,122 @@
       <c r="AA6" s="1" t="n"/>
     </row>
     <row r="7" ht="22.5" customHeight="1">
-      <c r="A7" s="41" t="inlineStr">
+      <c r="A7" s="99" t="inlineStr">
         <is>
           <t>RNC Nº</t>
         </is>
       </c>
-      <c r="B7" s="41" t="n">
-        <v>5417229751</v>
-      </c>
-      <c r="C7" s="41" t="inlineStr">
+      <c r="B7" s="99" t="n">
+        <v>5328477757</v>
+      </c>
+      <c r="C7" s="99" t="inlineStr">
         <is>
           <t>Origem:</t>
         </is>
       </c>
-      <c r="D7" s="43" t="inlineStr">
-        <is>
-          <t>Fornecedor</t>
-        </is>
-      </c>
-      <c r="E7" s="124" t="n"/>
-      <c r="F7" s="44" t="n"/>
-      <c r="G7" s="38" t="n"/>
-      <c r="H7" s="44" t="inlineStr">
+      <c r="D7" s="100" t="inlineStr">
+        <is>
+          <t>Corte e Estamparia</t>
+        </is>
+      </c>
+      <c r="E7" s="121" t="n"/>
+      <c r="F7" s="76" t="n"/>
+      <c r="G7" s="97" t="n"/>
+      <c r="H7" s="76" t="inlineStr">
         <is>
           <t>Data:</t>
         </is>
       </c>
       <c r="I7" s="12" t="inlineStr">
         <is>
-          <t>17/07/2023</t>
+          <t>06/10/2023</t>
         </is>
       </c>
       <c r="L7" s="2" t="n"/>
     </row>
     <row r="8" ht="18" customHeight="1">
-      <c r="A8" s="125" t="n"/>
-      <c r="B8" s="125" t="n"/>
-      <c r="C8" s="125" t="n"/>
-      <c r="D8" s="126" t="n"/>
-      <c r="E8" s="127" t="n"/>
-      <c r="F8" s="44" t="inlineStr">
+      <c r="A8" s="122" t="n"/>
+      <c r="B8" s="122" t="n"/>
+      <c r="C8" s="122" t="n"/>
+      <c r="D8" s="123" t="n"/>
+      <c r="E8" s="124" t="n"/>
+      <c r="F8" s="76" t="inlineStr">
         <is>
           <t>Resp.:</t>
         </is>
       </c>
-      <c r="G8" s="38" t="inlineStr">
-        <is>
-          <t>Severiano Neto, lauriene@cemag.com.br</t>
-        </is>
-      </c>
-      <c r="H8" s="122" t="n"/>
-      <c r="I8" s="123" t="n"/>
+      <c r="G8" s="97" t="inlineStr">
+        <is>
+          <t>abdias@cemag.com.br</t>
+        </is>
+      </c>
+      <c r="H8" s="119" t="n"/>
+      <c r="I8" s="120" t="n"/>
     </row>
     <row r="9" ht="22.5" customHeight="1">
-      <c r="A9" s="44" t="inlineStr">
+      <c r="A9" s="76" t="inlineStr">
         <is>
           <t>Descrição do Problema</t>
         </is>
       </c>
-      <c r="B9" s="122" t="n"/>
-      <c r="C9" s="122" t="n"/>
-      <c r="D9" s="122" t="n"/>
-      <c r="E9" s="122" t="n"/>
-      <c r="F9" s="122" t="n"/>
-      <c r="G9" s="122" t="n"/>
-      <c r="H9" s="122" t="n"/>
-      <c r="I9" s="123" t="n"/>
-    </row>
-    <row r="10" ht="18.75" customHeight="1">
-      <c r="A10" s="45" t="inlineStr">
-        <is>
-          <t>07/07/2023
-Cubos de roda referentes ao pedido de NF Nº. 000.037.127, apresentando dificuldade de montagem dos parafuso de roda no processo de fixação dos mesmo feito pelo almoxarifado. Uma amostra de cubo chegou a tricar devido a aplicação de força da máquina na tentativa de fixação.</t>
-        </is>
-      </c>
-      <c r="B10" s="128" t="n"/>
-      <c r="C10" s="128" t="n"/>
-      <c r="D10" s="128" t="n"/>
-      <c r="E10" s="128" t="n"/>
-      <c r="F10" s="128" t="n"/>
-      <c r="G10" s="128" t="n"/>
-      <c r="H10" s="128" t="n"/>
-      <c r="I10" s="124" t="n"/>
-    </row>
-    <row r="11" ht="18.75" customHeight="1">
-      <c r="A11" s="126" t="n"/>
-      <c r="B11" s="129" t="n"/>
-      <c r="C11" s="129" t="n"/>
-      <c r="D11" s="129" t="n"/>
-      <c r="E11" s="129" t="n"/>
-      <c r="F11" s="129" t="n"/>
-      <c r="G11" s="129" t="n"/>
-      <c r="H11" s="129" t="n"/>
-      <c r="I11" s="127" t="n"/>
+      <c r="B9" s="119" t="n"/>
+      <c r="C9" s="119" t="n"/>
+      <c r="D9" s="119" t="n"/>
+      <c r="E9" s="119" t="n"/>
+      <c r="F9" s="119" t="n"/>
+      <c r="G9" s="119" t="n"/>
+      <c r="H9" s="119" t="n"/>
+      <c r="I9" s="120" t="n"/>
+    </row>
+    <row r="10" ht="24.95" customHeight="1">
+      <c r="A10" s="82" t="inlineStr">
+        <is>
+          <t>No dia 06/10/2023 foram produzidas 80 que tem por código 025546 - FECHAM EIXO F4 (NOV13...) apresentando medida de virada 10mm menor.</t>
+        </is>
+      </c>
+      <c r="B10" s="125" t="n"/>
+      <c r="C10" s="125" t="n"/>
+      <c r="D10" s="125" t="n"/>
+      <c r="E10" s="125" t="n"/>
+      <c r="F10" s="125" t="n"/>
+      <c r="G10" s="125" t="n"/>
+      <c r="H10" s="125" t="n"/>
+      <c r="I10" s="121" t="n"/>
+    </row>
+    <row r="11" ht="24.95" customHeight="1">
+      <c r="A11" s="123" t="n"/>
+      <c r="B11" s="126" t="n"/>
+      <c r="C11" s="126" t="n"/>
+      <c r="D11" s="126" t="n"/>
+      <c r="E11" s="126" t="n"/>
+      <c r="F11" s="126" t="n"/>
+      <c r="G11" s="126" t="n"/>
+      <c r="H11" s="126" t="n"/>
+      <c r="I11" s="124" t="n"/>
     </row>
     <row r="12" ht="18.75" customHeight="1">
-      <c r="A12" s="48" t="n"/>
-      <c r="B12" s="128" t="n"/>
-      <c r="C12" s="128" t="n"/>
-      <c r="D12" s="128" t="n"/>
-      <c r="E12" s="128" t="n"/>
-      <c r="F12" s="128" t="n"/>
-      <c r="G12" s="128" t="n"/>
-      <c r="H12" s="128" t="n"/>
-      <c r="I12" s="128" t="n"/>
+      <c r="A12" s="87" t="n"/>
+      <c r="B12" s="125" t="n"/>
+      <c r="C12" s="125" t="n"/>
+      <c r="D12" s="125" t="n"/>
+      <c r="E12" s="125" t="n"/>
+      <c r="F12" s="125" t="n"/>
+      <c r="G12" s="125" t="n"/>
+      <c r="H12" s="125" t="n"/>
+      <c r="I12" s="125" t="n"/>
     </row>
     <row r="13" ht="23.25" customHeight="1">
-      <c r="A13" s="50" t="inlineStr">
+      <c r="A13" s="83" t="inlineStr">
         <is>
           <t>2ª ETAPA - AÇÃO IMEDIATA</t>
         </is>
       </c>
-      <c r="B13" s="111" t="n"/>
-      <c r="C13" s="111" t="n"/>
-      <c r="D13" s="111" t="n"/>
-      <c r="E13" s="121" t="n"/>
+      <c r="B13" s="108" t="n"/>
+      <c r="C13" s="108" t="n"/>
+      <c r="D13" s="108" t="n"/>
+      <c r="E13" s="118" t="n"/>
       <c r="F13" s="13" t="n"/>
-      <c r="G13" s="38" t="n"/>
+      <c r="G13" s="97" t="n"/>
       <c r="H13" s="13" t="inlineStr">
         <is>
           <t>Data</t>
@@ -1909,77 +1899,77 @@
       </c>
       <c r="I13" s="12" t="inlineStr">
         <is>
-          <t>17/07/2023</t>
+          <t>06/10/2023</t>
         </is>
       </c>
     </row>
     <row r="14" ht="22.5" customHeight="1">
-      <c r="A14" s="130" t="n"/>
-      <c r="B14" s="131" t="n"/>
-      <c r="C14" s="131" t="n"/>
-      <c r="D14" s="131" t="n"/>
-      <c r="E14" s="132" t="n"/>
+      <c r="A14" s="127" t="n"/>
+      <c r="B14" s="128" t="n"/>
+      <c r="C14" s="128" t="n"/>
+      <c r="D14" s="128" t="n"/>
+      <c r="E14" s="129" t="n"/>
       <c r="F14" s="14" t="inlineStr">
         <is>
           <t>Resp.:</t>
         </is>
       </c>
-      <c r="G14" s="53" t="inlineStr">
-        <is>
-          <t>Severiano Neto, lauriene@cemag.com.br</t>
-        </is>
-      </c>
-      <c r="H14" s="128" t="n"/>
-      <c r="I14" s="124" t="n"/>
+      <c r="G14" s="91" t="inlineStr">
+        <is>
+          <t>abdias@cemag.com.br</t>
+        </is>
+      </c>
+      <c r="H14" s="125" t="n"/>
+      <c r="I14" s="121" t="n"/>
     </row>
     <row r="15" ht="22.5" customHeight="1">
-      <c r="A15" s="44" t="inlineStr">
+      <c r="A15" s="76" t="inlineStr">
         <is>
           <t>Ação imediata</t>
         </is>
       </c>
-      <c r="B15" s="122" t="n"/>
-      <c r="C15" s="122" t="n"/>
-      <c r="D15" s="122" t="n"/>
-      <c r="E15" s="122" t="n"/>
-      <c r="F15" s="122" t="n"/>
-      <c r="G15" s="122" t="n"/>
-      <c r="H15" s="122" t="n"/>
-      <c r="I15" s="123" t="n"/>
+      <c r="B15" s="119" t="n"/>
+      <c r="C15" s="119" t="n"/>
+      <c r="D15" s="119" t="n"/>
+      <c r="E15" s="119" t="n"/>
+      <c r="F15" s="119" t="n"/>
+      <c r="G15" s="119" t="n"/>
+      <c r="H15" s="119" t="n"/>
+      <c r="I15" s="120" t="n"/>
     </row>
     <row r="16" ht="27.95" customHeight="1">
-      <c r="A16" s="45" t="inlineStr">
-        <is>
-          <t>Cortar relações com fornecedor Fundição BB, segregar material e informar que só pode ser usado em cbhm4500 mediante reabertura dos furos.</t>
-        </is>
-      </c>
-      <c r="B16" s="128" t="n"/>
-      <c r="C16" s="128" t="n"/>
-      <c r="D16" s="128" t="n"/>
-      <c r="E16" s="128" t="n"/>
-      <c r="F16" s="128" t="n"/>
-      <c r="G16" s="128" t="n"/>
-      <c r="H16" s="128" t="n"/>
-      <c r="I16" s="124" t="n"/>
+      <c r="A16" s="82" t="inlineStr">
+        <is>
+          <t>Inspetor Gutemberg no dia 06/10/2023 realizou retrabalho das 80 peças utilizando calandra para desfazer a virada e as peças retornaram para serem viradas na produção.</t>
+        </is>
+      </c>
+      <c r="B16" s="125" t="n"/>
+      <c r="C16" s="125" t="n"/>
+      <c r="D16" s="125" t="n"/>
+      <c r="E16" s="125" t="n"/>
+      <c r="F16" s="125" t="n"/>
+      <c r="G16" s="125" t="n"/>
+      <c r="H16" s="125" t="n"/>
+      <c r="I16" s="121" t="n"/>
     </row>
     <row r="17" ht="27.95" customHeight="1">
-      <c r="A17" s="133" t="n"/>
-      <c r="I17" s="134" t="n"/>
+      <c r="A17" s="130" t="n"/>
+      <c r="I17" s="131" t="n"/>
     </row>
     <row r="18" ht="27.95" customHeight="1">
-      <c r="A18" s="133" t="n"/>
-      <c r="I18" s="134" t="n"/>
+      <c r="A18" s="130" t="n"/>
+      <c r="I18" s="131" t="n"/>
     </row>
     <row r="19" ht="23.25" customHeight="1">
-      <c r="A19" s="126" t="n"/>
-      <c r="B19" s="129" t="n"/>
-      <c r="C19" s="129" t="n"/>
-      <c r="D19" s="129" t="n"/>
-      <c r="E19" s="129" t="n"/>
-      <c r="F19" s="129" t="n"/>
-      <c r="G19" s="129" t="n"/>
-      <c r="H19" s="129" t="n"/>
-      <c r="I19" s="127" t="n"/>
+      <c r="A19" s="123" t="n"/>
+      <c r="B19" s="126" t="n"/>
+      <c r="C19" s="126" t="n"/>
+      <c r="D19" s="126" t="n"/>
+      <c r="E19" s="126" t="n"/>
+      <c r="F19" s="126" t="n"/>
+      <c r="G19" s="126" t="n"/>
+      <c r="H19" s="126" t="n"/>
+      <c r="I19" s="124" t="n"/>
       <c r="J19" s="1" t="n"/>
       <c r="K19" s="1" t="n"/>
       <c r="L19" s="1" t="n"/>
@@ -2000,64 +1990,68 @@
       <c r="AA19" s="1" t="n"/>
     </row>
     <row r="20" ht="18.75" customHeight="1">
-      <c r="A20" s="98" t="n"/>
-      <c r="B20" s="131" t="n"/>
-      <c r="C20" s="131" t="n"/>
-      <c r="D20" s="131" t="n"/>
-      <c r="E20" s="131" t="n"/>
-      <c r="F20" s="131" t="n"/>
-      <c r="G20" s="131" t="n"/>
-      <c r="H20" s="131" t="n"/>
-      <c r="I20" s="132" t="n"/>
+      <c r="A20" s="79" t="n"/>
+      <c r="B20" s="128" t="n"/>
+      <c r="C20" s="128" t="n"/>
+      <c r="D20" s="128" t="n"/>
+      <c r="E20" s="128" t="n"/>
+      <c r="F20" s="128" t="n"/>
+      <c r="G20" s="128" t="n"/>
+      <c r="H20" s="128" t="n"/>
+      <c r="I20" s="129" t="n"/>
     </row>
     <row r="21" ht="23.25" customHeight="1">
-      <c r="A21" s="50" t="inlineStr">
+      <c r="A21" s="83" t="inlineStr">
         <is>
           <t>3ª ETAPA - ANÁLISE DE CAUZA RAIZ</t>
         </is>
       </c>
-      <c r="B21" s="111" t="n"/>
-      <c r="C21" s="111" t="n"/>
-      <c r="D21" s="111" t="n"/>
-      <c r="E21" s="121" t="n"/>
+      <c r="B21" s="108" t="n"/>
+      <c r="C21" s="108" t="n"/>
+      <c r="D21" s="108" t="n"/>
+      <c r="E21" s="118" t="n"/>
       <c r="F21" s="17" t="inlineStr">
         <is>
           <t>Data:</t>
         </is>
       </c>
-      <c r="G21" s="108" t="n">
-        <v/>
-      </c>
-      <c r="H21" s="135" t="n"/>
-      <c r="I21" s="112" t="n"/>
+      <c r="G21" s="23" t="inlineStr">
+        <is>
+          <t>13/10/2023</t>
+        </is>
+      </c>
+      <c r="H21" s="132" t="n"/>
+      <c r="I21" s="109" t="n"/>
     </row>
     <row r="22" ht="18.75" customHeight="1">
-      <c r="A22" s="130" t="n"/>
-      <c r="B22" s="131" t="n"/>
-      <c r="C22" s="131" t="n"/>
-      <c r="D22" s="131" t="n"/>
-      <c r="E22" s="132" t="n"/>
-      <c r="F22" s="66" t="n"/>
-      <c r="G22" s="136" t="n"/>
-      <c r="H22" s="117" t="n"/>
-      <c r="I22" s="118" t="n"/>
+      <c r="A22" s="127" t="n"/>
+      <c r="B22" s="128" t="n"/>
+      <c r="C22" s="128" t="n"/>
+      <c r="D22" s="128" t="n"/>
+      <c r="E22" s="129" t="n"/>
+      <c r="F22" s="74" t="n"/>
+      <c r="G22" s="133" t="n"/>
+      <c r="H22" s="114" t="n"/>
+      <c r="I22" s="115" t="n"/>
     </row>
     <row r="23" ht="45" customHeight="1">
-      <c r="A23" s="104" t="inlineStr">
+      <c r="A23" s="8" t="inlineStr">
         <is>
           <t>Máquina</t>
         </is>
       </c>
-      <c r="B23" s="105" t="n">
-        <v/>
-      </c>
-      <c r="C23" s="137" t="n"/>
-      <c r="D23" s="137" t="n"/>
-      <c r="E23" s="137" t="n"/>
-      <c r="F23" s="137" t="n"/>
-      <c r="G23" s="137" t="n"/>
-      <c r="H23" s="137" t="n"/>
-      <c r="I23" s="138" t="n"/>
+      <c r="B23" s="84" t="inlineStr">
+        <is>
+          <t>Virada realizada na viradeira 4, como de costume.</t>
+        </is>
+      </c>
+      <c r="C23" s="134" t="n"/>
+      <c r="D23" s="134" t="n"/>
+      <c r="E23" s="134" t="n"/>
+      <c r="F23" s="134" t="n"/>
+      <c r="G23" s="134" t="n"/>
+      <c r="H23" s="134" t="n"/>
+      <c r="I23" s="135" t="n"/>
     </row>
     <row r="24" ht="45" customHeight="1">
       <c r="A24" s="8" t="inlineStr">
@@ -2065,16 +2059,18 @@
           <t>Mão-de-Obra</t>
         </is>
       </c>
-      <c r="B24" s="59" t="n">
-        <v/>
-      </c>
-      <c r="C24" s="137" t="n"/>
-      <c r="D24" s="137" t="n"/>
-      <c r="E24" s="137" t="n"/>
-      <c r="F24" s="137" t="n"/>
-      <c r="G24" s="137" t="n"/>
-      <c r="H24" s="137" t="n"/>
-      <c r="I24" s="138" t="n"/>
+      <c r="B24" s="63" t="inlineStr">
+        <is>
+          <t>Colaborador que realizou a virada foi Célio (Gato a Jato), esse colaborador não é um operador treinado, ele é um ajudante.</t>
+        </is>
+      </c>
+      <c r="C24" s="134" t="n"/>
+      <c r="D24" s="134" t="n"/>
+      <c r="E24" s="134" t="n"/>
+      <c r="F24" s="134" t="n"/>
+      <c r="G24" s="134" t="n"/>
+      <c r="H24" s="134" t="n"/>
+      <c r="I24" s="135" t="n"/>
     </row>
     <row r="25" ht="45" customHeight="1">
       <c r="A25" s="8" t="inlineStr">
@@ -2082,16 +2078,18 @@
           <t>Matéria Prima</t>
         </is>
       </c>
-      <c r="B25" s="59" t="n">
-        <v/>
-      </c>
-      <c r="C25" s="137" t="n"/>
-      <c r="D25" s="137" t="n"/>
-      <c r="E25" s="137" t="n"/>
-      <c r="F25" s="137" t="n"/>
-      <c r="G25" s="137" t="n"/>
-      <c r="H25" s="137" t="n"/>
-      <c r="I25" s="138" t="n"/>
+      <c r="B25" s="63" t="inlineStr">
+        <is>
+          <t>Medidas da peça cortada estavam corformes.</t>
+        </is>
+      </c>
+      <c r="C25" s="134" t="n"/>
+      <c r="D25" s="134" t="n"/>
+      <c r="E25" s="134" t="n"/>
+      <c r="F25" s="134" t="n"/>
+      <c r="G25" s="134" t="n"/>
+      <c r="H25" s="134" t="n"/>
+      <c r="I25" s="135" t="n"/>
     </row>
     <row r="26" ht="45" customHeight="1">
       <c r="A26" s="8" t="inlineStr">
@@ -2099,16 +2097,18 @@
           <t>Medição</t>
         </is>
       </c>
-      <c r="B26" s="59" t="n">
-        <v/>
-      </c>
-      <c r="C26" s="137" t="n"/>
-      <c r="D26" s="137" t="n"/>
-      <c r="E26" s="137" t="n"/>
-      <c r="F26" s="137" t="n"/>
-      <c r="G26" s="137" t="n"/>
-      <c r="H26" s="137" t="n"/>
-      <c r="I26" s="138" t="n"/>
+      <c r="B26" s="63" t="inlineStr">
+        <is>
+          <t>Operador possui uma trena em pessima condições, com graduações descascando e nao estando no plano de calibração.</t>
+        </is>
+      </c>
+      <c r="C26" s="134" t="n"/>
+      <c r="D26" s="134" t="n"/>
+      <c r="E26" s="134" t="n"/>
+      <c r="F26" s="134" t="n"/>
+      <c r="G26" s="134" t="n"/>
+      <c r="H26" s="134" t="n"/>
+      <c r="I26" s="135" t="n"/>
     </row>
     <row r="27" ht="45" customHeight="1">
       <c r="A27" s="8" t="inlineStr">
@@ -2116,16 +2116,18 @@
           <t>Método</t>
         </is>
       </c>
-      <c r="B27" s="59" t="n">
-        <v/>
-      </c>
-      <c r="C27" s="137" t="n"/>
-      <c r="D27" s="137" t="n"/>
-      <c r="E27" s="137" t="n"/>
-      <c r="F27" s="137" t="n"/>
-      <c r="G27" s="137" t="n"/>
-      <c r="H27" s="137" t="n"/>
-      <c r="I27" s="138" t="n"/>
+      <c r="B27" s="63" t="inlineStr">
+        <is>
+          <t>O supervisor ao repassar a  atividade informou sobre o gabarito na viradeira a qual a peça deveria encostar para realizar a virada.</t>
+        </is>
+      </c>
+      <c r="C27" s="134" t="n"/>
+      <c r="D27" s="134" t="n"/>
+      <c r="E27" s="134" t="n"/>
+      <c r="F27" s="134" t="n"/>
+      <c r="G27" s="134" t="n"/>
+      <c r="H27" s="134" t="n"/>
+      <c r="I27" s="135" t="n"/>
     </row>
     <row r="28" ht="45" customHeight="1">
       <c r="A28" s="8" t="inlineStr">
@@ -2133,59 +2135,61 @@
           <t>Meio Ambiente</t>
         </is>
       </c>
-      <c r="B28" s="59" t="n">
+      <c r="B28" s="63" t="n">
         <v/>
       </c>
-      <c r="C28" s="137" t="n"/>
-      <c r="D28" s="137" t="n"/>
-      <c r="E28" s="137" t="n"/>
-      <c r="F28" s="137" t="n"/>
-      <c r="G28" s="137" t="n"/>
-      <c r="H28" s="137" t="n"/>
-      <c r="I28" s="138" t="n"/>
+      <c r="C28" s="134" t="n"/>
+      <c r="D28" s="134" t="n"/>
+      <c r="E28" s="134" t="n"/>
+      <c r="F28" s="134" t="n"/>
+      <c r="G28" s="134" t="n"/>
+      <c r="H28" s="134" t="n"/>
+      <c r="I28" s="135" t="n"/>
     </row>
     <row r="29" ht="45" customHeight="1">
-      <c r="A29" s="68" t="inlineStr">
+      <c r="A29" s="66" t="inlineStr">
         <is>
           <t>Presentes:</t>
         </is>
       </c>
-      <c r="B29" s="139" t="n"/>
-      <c r="C29" s="69" t="n">
-        <v/>
-      </c>
-      <c r="D29" s="136" t="n"/>
-      <c r="E29" s="136" t="n"/>
-      <c r="F29" s="136" t="n"/>
-      <c r="G29" s="136" t="n"/>
-      <c r="H29" s="136" t="n"/>
-      <c r="I29" s="139" t="n"/>
+      <c r="B29" s="136" t="n"/>
+      <c r="C29" s="68" t="inlineStr">
+        <is>
+          <t>Estefane, Severiano, Guthemberg</t>
+        </is>
+      </c>
+      <c r="D29" s="133" t="n"/>
+      <c r="E29" s="133" t="n"/>
+      <c r="F29" s="133" t="n"/>
+      <c r="G29" s="133" t="n"/>
+      <c r="H29" s="133" t="n"/>
+      <c r="I29" s="136" t="n"/>
     </row>
     <row r="30" ht="6" customHeight="1">
-      <c r="A30" s="56" t="n"/>
-      <c r="B30" s="140" t="n"/>
-      <c r="C30" s="140" t="n"/>
-      <c r="D30" s="140" t="n"/>
-      <c r="E30" s="140" t="n"/>
-      <c r="F30" s="140" t="n"/>
-      <c r="G30" s="140" t="n"/>
-      <c r="H30" s="140" t="n"/>
-      <c r="I30" s="141" t="n"/>
+      <c r="A30" s="24" t="n"/>
+      <c r="B30" s="137" t="n"/>
+      <c r="C30" s="137" t="n"/>
+      <c r="D30" s="137" t="n"/>
+      <c r="E30" s="137" t="n"/>
+      <c r="F30" s="137" t="n"/>
+      <c r="G30" s="137" t="n"/>
+      <c r="H30" s="137" t="n"/>
+      <c r="I30" s="138" t="n"/>
     </row>
     <row r="31" ht="36.75" customHeight="1">
-      <c r="A31" s="72" t="inlineStr">
+      <c r="A31" s="52" t="inlineStr">
         <is>
           <t>3ªETAPA - PLANO DE AÇÃO</t>
         </is>
       </c>
-      <c r="B31" s="137" t="n"/>
-      <c r="C31" s="137" t="n"/>
-      <c r="D31" s="137" t="n"/>
-      <c r="E31" s="137" t="n"/>
-      <c r="F31" s="137" t="n"/>
-      <c r="G31" s="137" t="n"/>
-      <c r="H31" s="137" t="n"/>
-      <c r="I31" s="138" t="n"/>
+      <c r="B31" s="134" t="n"/>
+      <c r="C31" s="134" t="n"/>
+      <c r="D31" s="134" t="n"/>
+      <c r="E31" s="134" t="n"/>
+      <c r="F31" s="134" t="n"/>
+      <c r="G31" s="134" t="n"/>
+      <c r="H31" s="134" t="n"/>
+      <c r="I31" s="135" t="n"/>
       <c r="J31" s="1" t="n"/>
       <c r="K31" s="1" t="n"/>
       <c r="L31" s="1" t="n"/>
@@ -2206,356 +2210,379 @@
       <c r="AA31" s="1" t="n"/>
     </row>
     <row r="32" ht="18.75" customHeight="1">
-      <c r="A32" s="74" t="inlineStr">
+      <c r="A32" s="53" t="inlineStr">
         <is>
           <t>Atividade</t>
         </is>
       </c>
-      <c r="B32" s="111" t="n"/>
-      <c r="C32" s="111" t="n"/>
-      <c r="D32" s="121" t="n"/>
-      <c r="E32" s="75" t="inlineStr">
+      <c r="B32" s="108" t="n"/>
+      <c r="C32" s="108" t="n"/>
+      <c r="D32" s="118" t="n"/>
+      <c r="E32" s="55" t="inlineStr">
         <is>
           <t>Responsável</t>
         </is>
       </c>
-      <c r="F32" s="142" t="inlineStr">
+      <c r="F32" s="139" t="inlineStr">
         <is>
           <t>Executor</t>
         </is>
       </c>
-      <c r="G32" s="143" t="n"/>
-      <c r="H32" s="144" t="inlineStr">
+      <c r="G32" s="140" t="n"/>
+      <c r="H32" s="141" t="inlineStr">
         <is>
           <t>Previsão</t>
         </is>
       </c>
-      <c r="I32" s="144" t="inlineStr">
+      <c r="I32" s="141" t="inlineStr">
         <is>
           <t>Realizado</t>
         </is>
       </c>
     </row>
     <row r="33" ht="9" customHeight="1">
-      <c r="A33" s="130" t="n"/>
-      <c r="B33" s="131" t="n"/>
-      <c r="C33" s="131" t="n"/>
-      <c r="D33" s="132" t="n"/>
-      <c r="E33" s="145" t="n"/>
-      <c r="F33" s="146" t="n"/>
-      <c r="G33" s="134" t="n"/>
-      <c r="H33" s="125" t="n"/>
-      <c r="I33" s="125" t="n"/>
+      <c r="A33" s="127" t="n"/>
+      <c r="B33" s="128" t="n"/>
+      <c r="C33" s="128" t="n"/>
+      <c r="D33" s="129" t="n"/>
+      <c r="E33" s="142" t="n"/>
+      <c r="F33" s="143" t="n"/>
+      <c r="G33" s="131" t="n"/>
+      <c r="H33" s="122" t="n"/>
+      <c r="I33" s="122" t="n"/>
     </row>
     <row r="34" ht="28.5" customHeight="1">
-      <c r="A34" s="82" t="inlineStr">
-        <is>
-          <t>Realizar ensaios necessáruos</t>
-        </is>
-      </c>
-      <c r="B34" s="136" t="n"/>
-      <c r="C34" s="136" t="n"/>
-      <c r="D34" s="139" t="n"/>
+      <c r="A34" s="38" t="inlineStr">
+        <is>
+          <t>Entregar trena calibrada para o colaborador.</t>
+        </is>
+      </c>
+      <c r="B34" s="133" t="n"/>
+      <c r="C34" s="133" t="n"/>
+      <c r="D34" s="136" t="n"/>
       <c r="E34" s="9" t="inlineStr">
         <is>
-          <t>Severiano Neto</t>
-        </is>
-      </c>
-      <c r="F34" s="147" t="inlineStr">
-        <is>
-          <t>Severiano</t>
-        </is>
-      </c>
-      <c r="G34" s="123" t="n"/>
+          <t>Estefane Santos</t>
+        </is>
+      </c>
+      <c r="F34" s="144" t="inlineStr">
+        <is>
+          <t>Estefane</t>
+        </is>
+      </c>
+      <c r="G34" s="120" t="n"/>
       <c r="H34" s="18" t="inlineStr">
         <is>
-          <t>07/07/2023</t>
+          <t>16/10/2023</t>
         </is>
       </c>
       <c r="I34" s="18" t="n">
-        <v>45118</v>
+        <v>45216</v>
       </c>
     </row>
     <row r="35" ht="28.5" customHeight="1">
-      <c r="A35" s="82" t="inlineStr">
-        <is>
-          <t>Repassar problemática para fornecedor</t>
-        </is>
-      </c>
-      <c r="B35" s="136" t="n"/>
-      <c r="C35" s="136" t="n"/>
-      <c r="D35" s="139" t="n"/>
+      <c r="A35" s="38" t="inlineStr">
+        <is>
+          <t>Reforçar com inspetor da área a importancia do acompanhamento das atividades que forem exercidas pela 1° Vez</t>
+        </is>
+      </c>
+      <c r="B35" s="133" t="n"/>
+      <c r="C35" s="133" t="n"/>
+      <c r="D35" s="136" t="n"/>
       <c r="E35" s="9" t="inlineStr">
         <is>
-          <t>lauriene@cemag.com.br</t>
-        </is>
-      </c>
-      <c r="F35" s="147" t="inlineStr">
-        <is>
-          <t>Lauriene</t>
-        </is>
-      </c>
-      <c r="G35" s="123" t="n"/>
+          <t>Estefane Santos</t>
+        </is>
+      </c>
+      <c r="F35" s="144" t="inlineStr">
+        <is>
+          <t>Estefane</t>
+        </is>
+      </c>
+      <c r="G35" s="120" t="n"/>
       <c r="H35" s="18" t="inlineStr">
         <is>
-          <t>17/07/2023</t>
+          <t>17/10/2023</t>
         </is>
       </c>
       <c r="I35" s="18" t="n">
-        <v>45124</v>
+        <v>45216</v>
       </c>
     </row>
     <row r="36" ht="28.5" customHeight="1">
-      <c r="A36" s="82" t="inlineStr">
-        <is>
-          <t>Segregar e identificar material</t>
-        </is>
-      </c>
-      <c r="B36" s="136" t="n"/>
-      <c r="C36" s="136" t="n"/>
-      <c r="D36" s="139" t="n"/>
+      <c r="A36" s="38" t="inlineStr">
+        <is>
+          <t>Alinhar com a Supervisão que a atividade de virada não pode ser realizada por um ajudante não treinado</t>
+        </is>
+      </c>
+      <c r="B36" s="133" t="n"/>
+      <c r="C36" s="133" t="n"/>
+      <c r="D36" s="136" t="n"/>
       <c r="E36" s="9" t="inlineStr">
         <is>
-          <t>Estefane Santos</t>
-        </is>
-      </c>
-      <c r="F36" s="147" t="inlineStr">
-        <is>
-          <t>Estefane</t>
-        </is>
-      </c>
-      <c r="G36" s="123" t="n"/>
+          <t>Severiano Neto, Estefane Santos</t>
+        </is>
+      </c>
+      <c r="F36" s="144" t="inlineStr">
+        <is>
+          <t>Alex, Severiano, Estefane, Guthemberg</t>
+        </is>
+      </c>
+      <c r="G36" s="120" t="n"/>
       <c r="H36" s="18" t="inlineStr">
         <is>
-          <t>17/07/2023</t>
+          <t>17/10/2023</t>
         </is>
       </c>
       <c r="I36" s="18" t="n">
-        <v>45229</v>
+        <v>45238</v>
       </c>
     </row>
     <row r="37" ht="28.5" customHeight="1">
-      <c r="A37" s="82" t="inlineStr"/>
-      <c r="B37" s="136" t="n"/>
-      <c r="C37" s="136" t="n"/>
-      <c r="D37" s="139" t="n"/>
+      <c r="A37" s="38" t="inlineStr"/>
+      <c r="B37" s="133" t="n"/>
+      <c r="C37" s="133" t="n"/>
+      <c r="D37" s="136" t="n"/>
       <c r="E37" s="9" t="inlineStr"/>
-      <c r="F37" s="147" t="inlineStr"/>
-      <c r="G37" s="123" t="n"/>
+      <c r="F37" s="144" t="inlineStr"/>
+      <c r="G37" s="120" t="n"/>
       <c r="H37" s="18" t="inlineStr"/>
       <c r="I37" s="18" t="inlineStr"/>
     </row>
     <row r="38" ht="28.5" customHeight="1">
-      <c r="A38" s="82" t="n"/>
-      <c r="B38" s="136" t="n"/>
-      <c r="C38" s="136" t="n"/>
-      <c r="D38" s="139" t="n"/>
+      <c r="A38" s="38" t="n"/>
+      <c r="B38" s="133" t="n"/>
+      <c r="C38" s="133" t="n"/>
+      <c r="D38" s="136" t="n"/>
       <c r="E38" s="9" t="n"/>
-      <c r="F38" s="147" t="n"/>
-      <c r="G38" s="123" t="n"/>
+      <c r="F38" s="144" t="n"/>
+      <c r="G38" s="120" t="n"/>
       <c r="H38" s="18" t="n"/>
       <c r="I38" s="18" t="n"/>
     </row>
-    <row r="39" ht="6" customHeight="1">
-      <c r="A39" s="89" t="n"/>
-      <c r="B39" s="136" t="n"/>
-      <c r="C39" s="136" t="n"/>
+    <row r="39" ht="28.5" customHeight="1">
+      <c r="A39" s="38" t="n"/>
+      <c r="B39" s="133" t="n"/>
+      <c r="C39" s="133" t="n"/>
       <c r="D39" s="136" t="n"/>
-      <c r="E39" s="136" t="n"/>
-      <c r="F39" s="136" t="n"/>
-      <c r="G39" s="136" t="n"/>
-      <c r="H39" s="136" t="n"/>
-      <c r="I39" s="139" t="n"/>
-    </row>
-    <row r="40" ht="18.75" customHeight="1">
-      <c r="A40" s="91" t="inlineStr">
+      <c r="E39" s="9" t="n"/>
+      <c r="F39" s="144" t="n"/>
+      <c r="G39" s="120" t="n"/>
+      <c r="H39" s="18" t="n"/>
+      <c r="I39" s="18" t="n"/>
+    </row>
+    <row r="40" ht="28.5" customHeight="1">
+      <c r="A40" s="38" t="n"/>
+      <c r="B40" s="133" t="n"/>
+      <c r="C40" s="133" t="n"/>
+      <c r="D40" s="136" t="n"/>
+      <c r="E40" s="9" t="n"/>
+      <c r="F40" s="144" t="n"/>
+      <c r="G40" s="120" t="n"/>
+      <c r="H40" s="18" t="n"/>
+      <c r="I40" s="18" t="n"/>
+    </row>
+    <row r="41" ht="28.5" customHeight="1">
+      <c r="A41" s="38" t="n"/>
+      <c r="B41" s="133" t="n"/>
+      <c r="C41" s="133" t="n"/>
+      <c r="D41" s="136" t="n"/>
+      <c r="E41" s="9" t="n"/>
+      <c r="F41" s="144" t="n"/>
+      <c r="G41" s="120" t="n"/>
+      <c r="H41" s="18" t="n"/>
+      <c r="I41" s="18" t="n"/>
+    </row>
+    <row r="42" ht="28.5" customHeight="1">
+      <c r="A42" s="38" t="n"/>
+      <c r="B42" s="133" t="n"/>
+      <c r="C42" s="133" t="n"/>
+      <c r="D42" s="136" t="n"/>
+      <c r="E42" s="9" t="n"/>
+      <c r="F42" s="144" t="n"/>
+      <c r="G42" s="120" t="n"/>
+      <c r="H42" s="18" t="n"/>
+      <c r="I42" s="18" t="n"/>
+    </row>
+    <row r="43" ht="28.5" customHeight="1">
+      <c r="A43" s="38" t="n"/>
+      <c r="B43" s="133" t="n"/>
+      <c r="C43" s="133" t="n"/>
+      <c r="D43" s="136" t="n"/>
+      <c r="E43" s="9" t="n"/>
+      <c r="F43" s="144" t="n"/>
+      <c r="G43" s="120" t="n"/>
+      <c r="H43" s="18" t="n"/>
+      <c r="I43" s="18" t="n"/>
+    </row>
+    <row r="44" ht="6" customHeight="1">
+      <c r="A44" s="43" t="n"/>
+      <c r="B44" s="133" t="n"/>
+      <c r="C44" s="133" t="n"/>
+      <c r="D44" s="133" t="n"/>
+      <c r="E44" s="133" t="n"/>
+      <c r="F44" s="133" t="n"/>
+      <c r="G44" s="133" t="n"/>
+      <c r="H44" s="133" t="n"/>
+      <c r="I44" s="136" t="n"/>
+    </row>
+    <row r="45" ht="18.75" customHeight="1">
+      <c r="A45" s="46" t="inlineStr">
         <is>
           <t>4ª ETAPA - EFICÁCIA</t>
         </is>
       </c>
-      <c r="B40" s="148" t="n"/>
-      <c r="C40" s="148" t="n"/>
-      <c r="D40" s="148" t="n"/>
-      <c r="E40" s="149" t="n"/>
-      <c r="F40" s="19" t="n"/>
-      <c r="G40" s="20" t="n"/>
-      <c r="H40" s="19" t="inlineStr">
+      <c r="B45" s="145" t="n"/>
+      <c r="C45" s="145" t="n"/>
+      <c r="D45" s="145" t="n"/>
+      <c r="E45" s="146" t="n"/>
+      <c r="F45" s="19" t="n"/>
+      <c r="G45" s="20" t="n"/>
+      <c r="H45" s="19" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
       </c>
-      <c r="I40" s="21" t="inlineStr">
-        <is>
-          <t>06/11/2023</t>
-        </is>
-      </c>
-    </row>
-    <row r="41" ht="18.75" customHeight="1">
-      <c r="A41" s="130" t="n"/>
-      <c r="B41" s="131" t="n"/>
-      <c r="C41" s="131" t="n"/>
-      <c r="D41" s="131" t="n"/>
-      <c r="E41" s="132" t="n"/>
-      <c r="F41" s="22" t="inlineStr">
+      <c r="I45" s="21" t="inlineStr"/>
+    </row>
+    <row r="46" ht="18.75" customHeight="1">
+      <c r="A46" s="127" t="n"/>
+      <c r="B46" s="128" t="n"/>
+      <c r="C46" s="128" t="n"/>
+      <c r="D46" s="128" t="n"/>
+      <c r="E46" s="129" t="n"/>
+      <c r="F46" s="22" t="inlineStr">
         <is>
           <t>Resp.:</t>
         </is>
       </c>
-      <c r="G41" s="93" t="inlineStr">
-        <is>
-          <t>Estefane Santos</t>
-        </is>
-      </c>
-      <c r="H41" s="140" t="n"/>
-      <c r="I41" s="141" t="n"/>
-    </row>
-    <row r="42" ht="25.5" customHeight="1">
-      <c r="A42" s="150" t="inlineStr">
+      <c r="G46" s="49" t="n">
+        <v/>
+      </c>
+      <c r="H46" s="137" t="n"/>
+      <c r="I46" s="138" t="n"/>
+    </row>
+    <row r="47" ht="25.5" customHeight="1">
+      <c r="A47" s="147" t="inlineStr">
         <is>
           <t>As ações corretivas foram eficazes? (Caso não, abrir nova RNC)</t>
         </is>
       </c>
-      <c r="B42" s="111" t="n"/>
-      <c r="C42" s="111" t="n"/>
-      <c r="D42" s="111" t="n"/>
-      <c r="E42" s="111" t="n"/>
-      <c r="F42" s="111" t="n"/>
-      <c r="G42" s="111" t="n"/>
-      <c r="H42" s="111" t="n"/>
-      <c r="I42" s="112" t="n"/>
-      <c r="J42" s="1" t="n"/>
-      <c r="K42" s="1" t="n"/>
-      <c r="L42" s="1" t="n"/>
-      <c r="M42" s="1" t="n"/>
-      <c r="N42" s="1" t="n"/>
-      <c r="O42" s="1" t="n"/>
-      <c r="P42" s="1" t="n"/>
-      <c r="Q42" s="1" t="n"/>
-      <c r="R42" s="1" t="n"/>
-      <c r="S42" s="1" t="n"/>
-      <c r="T42" s="1" t="n"/>
-      <c r="U42" s="1" t="n"/>
-      <c r="V42" s="1" t="n"/>
-      <c r="W42" s="1" t="n"/>
-      <c r="X42" s="1" t="n"/>
-      <c r="Y42" s="1" t="n"/>
-      <c r="Z42" s="1" t="n"/>
-      <c r="AA42" s="1" t="n"/>
-    </row>
-    <row r="43" ht="6" customHeight="1">
-      <c r="A43" s="56" t="n"/>
-      <c r="B43" s="140" t="n"/>
-      <c r="C43" s="140" t="n"/>
-      <c r="D43" s="140" t="n"/>
-      <c r="E43" s="140" t="n"/>
-      <c r="F43" s="140" t="n"/>
-      <c r="G43" s="140" t="n"/>
-      <c r="H43" s="140" t="n"/>
-      <c r="I43" s="141" t="n"/>
-    </row>
-    <row r="44" ht="36.75" customHeight="1">
-      <c r="A44" s="95" t="inlineStr">
+      <c r="B47" s="108" t="n"/>
+      <c r="C47" s="108" t="n"/>
+      <c r="D47" s="108" t="n"/>
+      <c r="E47" s="108" t="n"/>
+      <c r="F47" s="108" t="n"/>
+      <c r="G47" s="108" t="n"/>
+      <c r="H47" s="108" t="n"/>
+      <c r="I47" s="109" t="n"/>
+      <c r="J47" s="1" t="n"/>
+      <c r="K47" s="1" t="n"/>
+      <c r="L47" s="1" t="n"/>
+      <c r="M47" s="1" t="n"/>
+      <c r="N47" s="1" t="n"/>
+      <c r="O47" s="1" t="n"/>
+      <c r="P47" s="1" t="n"/>
+      <c r="Q47" s="1" t="n"/>
+      <c r="R47" s="1" t="n"/>
+      <c r="S47" s="1" t="n"/>
+      <c r="T47" s="1" t="n"/>
+      <c r="U47" s="1" t="n"/>
+      <c r="V47" s="1" t="n"/>
+      <c r="W47" s="1" t="n"/>
+      <c r="X47" s="1" t="n"/>
+      <c r="Y47" s="1" t="n"/>
+      <c r="Z47" s="1" t="n"/>
+      <c r="AA47" s="1" t="n"/>
+    </row>
+    <row r="48" ht="6" customHeight="1">
+      <c r="A48" s="24" t="n"/>
+      <c r="B48" s="137" t="n"/>
+      <c r="C48" s="137" t="n"/>
+      <c r="D48" s="137" t="n"/>
+      <c r="E48" s="137" t="n"/>
+      <c r="F48" s="137" t="n"/>
+      <c r="G48" s="137" t="n"/>
+      <c r="H48" s="137" t="n"/>
+      <c r="I48" s="138" t="n"/>
+    </row>
+    <row r="49" ht="36.75" customHeight="1">
+      <c r="A49" s="27" t="inlineStr">
         <is>
           <t>INFORMAÇÕES ADICIONAIS</t>
         </is>
       </c>
-      <c r="B44" s="137" t="n"/>
-      <c r="C44" s="137" t="n"/>
-      <c r="D44" s="137" t="n"/>
-      <c r="E44" s="137" t="n"/>
-      <c r="F44" s="137" t="n"/>
-      <c r="G44" s="137" t="n"/>
-      <c r="H44" s="137" t="n"/>
-      <c r="I44" s="138" t="n"/>
-      <c r="J44" s="1" t="n"/>
-      <c r="K44" s="1" t="n"/>
-      <c r="L44" s="1" t="n"/>
-      <c r="M44" s="1" t="n"/>
-      <c r="N44" s="1" t="n"/>
-      <c r="O44" s="1" t="n"/>
-      <c r="P44" s="1" t="n"/>
-      <c r="Q44" s="1" t="n"/>
-      <c r="R44" s="1" t="n"/>
-      <c r="S44" s="1" t="n"/>
-      <c r="T44" s="1" t="n"/>
-      <c r="U44" s="1" t="n"/>
-      <c r="V44" s="1" t="n"/>
-      <c r="W44" s="1" t="n"/>
-      <c r="X44" s="1" t="n"/>
-      <c r="Y44" s="1" t="n"/>
-      <c r="Z44" s="1" t="n"/>
-      <c r="AA44" s="1" t="n"/>
-    </row>
-    <row r="45" ht="42.75" customHeight="1">
-      <c r="A45" s="96">
-        <f>IF(H42="Não",VLOOKUP($B$7,#REF!,44),"")</f>
+      <c r="B49" s="134" t="n"/>
+      <c r="C49" s="134" t="n"/>
+      <c r="D49" s="134" t="n"/>
+      <c r="E49" s="134" t="n"/>
+      <c r="F49" s="134" t="n"/>
+      <c r="G49" s="134" t="n"/>
+      <c r="H49" s="134" t="n"/>
+      <c r="I49" s="135" t="n"/>
+      <c r="J49" s="1" t="n"/>
+      <c r="K49" s="1" t="n"/>
+      <c r="L49" s="1" t="n"/>
+      <c r="M49" s="1" t="n"/>
+      <c r="N49" s="1" t="n"/>
+      <c r="O49" s="1" t="n"/>
+      <c r="P49" s="1" t="n"/>
+      <c r="Q49" s="1" t="n"/>
+      <c r="R49" s="1" t="n"/>
+      <c r="S49" s="1" t="n"/>
+      <c r="T49" s="1" t="n"/>
+      <c r="U49" s="1" t="n"/>
+      <c r="V49" s="1" t="n"/>
+      <c r="W49" s="1" t="n"/>
+      <c r="X49" s="1" t="n"/>
+      <c r="Y49" s="1" t="n"/>
+      <c r="Z49" s="1" t="n"/>
+      <c r="AA49" s="1" t="n"/>
+    </row>
+    <row r="50" ht="42.75" customHeight="1">
+      <c r="A50" s="30">
+        <f>IF(H47="Não",VLOOKUP($B$7,#REF!,44),"")</f>
         <v/>
       </c>
-      <c r="B45" s="148" t="n"/>
-      <c r="C45" s="148" t="n"/>
-      <c r="D45" s="148" t="n"/>
-      <c r="E45" s="148" t="n"/>
-      <c r="F45" s="148" t="n"/>
-      <c r="G45" s="148" t="n"/>
-      <c r="H45" s="148" t="n"/>
-      <c r="I45" s="149" t="n"/>
-    </row>
-    <row r="46" ht="42.75" customHeight="1">
-      <c r="A46" s="130" t="n"/>
-      <c r="B46" s="131" t="n"/>
-      <c r="C46" s="131" t="n"/>
-      <c r="D46" s="131" t="n"/>
-      <c r="E46" s="131" t="n"/>
-      <c r="F46" s="131" t="n"/>
-      <c r="G46" s="131" t="n"/>
-      <c r="H46" s="131" t="n"/>
-      <c r="I46" s="132" t="n"/>
+      <c r="B50" s="145" t="n"/>
+      <c r="C50" s="145" t="n"/>
+      <c r="D50" s="145" t="n"/>
+      <c r="E50" s="145" t="n"/>
+      <c r="F50" s="145" t="n"/>
+      <c r="G50" s="145" t="n"/>
+      <c r="H50" s="145" t="n"/>
+      <c r="I50" s="146" t="n"/>
+    </row>
+    <row r="51" ht="42.75" customHeight="1">
+      <c r="A51" s="127" t="n"/>
+      <c r="B51" s="128" t="n"/>
+      <c r="C51" s="128" t="n"/>
+      <c r="D51" s="128" t="n"/>
+      <c r="E51" s="128" t="n"/>
+      <c r="F51" s="128" t="n"/>
+      <c r="G51" s="128" t="n"/>
+      <c r="H51" s="128" t="n"/>
+      <c r="I51" s="129" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="58">
-    <mergeCell ref="A43:I43"/>
-    <mergeCell ref="A44:I44"/>
-    <mergeCell ref="A45:I46"/>
-    <mergeCell ref="A42:I42"/>
+  <mergeCells count="68">
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="F37:G37"/>
     <mergeCell ref="A38:D38"/>
     <mergeCell ref="F38:G38"/>
-    <mergeCell ref="A39:I39"/>
-    <mergeCell ref="A40:E41"/>
-    <mergeCell ref="G41:I41"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="F37:G37"/>
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="F34:G34"/>
     <mergeCell ref="A35:D35"/>
     <mergeCell ref="F35:G35"/>
-    <mergeCell ref="A31:I31"/>
-    <mergeCell ref="A32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:G33"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="B27:I27"/>
-    <mergeCell ref="B28:I28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="A30:I30"/>
-    <mergeCell ref="B24:I24"/>
-    <mergeCell ref="B25:I25"/>
-    <mergeCell ref="H21:I22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="B26:I26"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="A20:I20"/>
-    <mergeCell ref="A16:I19"/>
-    <mergeCell ref="A21:E22"/>
-    <mergeCell ref="B23:I23"/>
-    <mergeCell ref="A9:I9"/>
-    <mergeCell ref="A10:I11"/>
-    <mergeCell ref="A12:I12"/>
-    <mergeCell ref="A13:E14"/>
-    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="B3:F4"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
     <mergeCell ref="A5:I5"/>
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="G6:I6"/>
@@ -2564,13 +2591,49 @@
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:E8"/>
     <mergeCell ref="G8:I8"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:F2"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="B3:F4"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="A10:I11"/>
+    <mergeCell ref="A12:I12"/>
+    <mergeCell ref="A13:E14"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="A20:I20"/>
+    <mergeCell ref="A16:I19"/>
+    <mergeCell ref="A21:E22"/>
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="B24:I24"/>
+    <mergeCell ref="B25:I25"/>
+    <mergeCell ref="H21:I22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="B26:I26"/>
+    <mergeCell ref="B27:I27"/>
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="A30:I30"/>
+    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="A32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:G33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="A48:I48"/>
+    <mergeCell ref="A49:I49"/>
+    <mergeCell ref="A50:I51"/>
+    <mergeCell ref="A47:I47"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="A44:I44"/>
+    <mergeCell ref="A45:E46"/>
+    <mergeCell ref="G46:I46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
formatacao nova no excel
</commit_message>
<xml_diff>
--- a/arquivo_formatado.xlsx
+++ b/arquivo_formatado.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="20370" yWindow="-1575" windowWidth="29040" windowHeight="16440" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="20370" yWindow="-1575" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RNCAC GQ-001-000" sheetId="1" state="visible" r:id="rId1"/>
@@ -60,12 +60,6 @@
     <font>
       <name val="Arial"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="16"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
       <color rgb="FFFF0000"/>
       <sz val="10"/>
     </font>
@@ -91,41 +85,46 @@
     <font>
       <name val="Arial"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <sz val="12"/>
     </font>
     <font>
       <name val="Arial"/>
       <family val="2"/>
       <color theme="1"/>
-      <sz val="16"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="14"/>
     </font>
     <font>
       <name val="Arial"/>
       <family val="2"/>
       <b val="1"/>
       <color rgb="FF000000"/>
-      <sz val="12"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="14"/>
     </font>
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="12"/>
+      <sz val="14"/>
     </font>
   </fonts>
   <fills count="8">
@@ -169,7 +168,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="83">
+  <borders count="88">
     <border>
       <left/>
       <right/>
@@ -420,30 +419,6 @@
         <color rgb="FF000000"/>
       </left>
       <right/>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -554,43 +529,6 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFC6C6C6"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFC6C6C6"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -902,6 +840,83 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC6C6C6"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFC6C6C6"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -926,18 +941,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
+      <left/>
+      <right style="thin">
+        <color rgb="FFC6C6C6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1061,15 +1072,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFC6C6C6"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1099,9 +1101,7 @@
       <right style="thin">
         <color rgb="FFC6C6C6"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -1132,30 +1132,74 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13"/>
   </cellStyleXfs>
-  <cellXfs count="196">
+  <cellXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -1184,8 +1228,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="60" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="58" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -1233,339 +1276,316 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="58" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="41" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="53" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="56" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="57" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="60" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="61" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="59" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="47" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="48" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="2" borderId="49" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="2" borderId="41" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="2" borderId="44" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="39" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="37" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="26" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="50" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="26" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="53" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="54" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="55" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="26" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="2" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="26" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="51" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="26" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="50" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="26" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="44" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="36" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="33" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="35" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="38" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="45" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="46" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="52" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="53" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="54" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="45" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="46" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="47" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="48" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="49" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="55" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="33" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="33" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="58" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="59" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="26" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="38" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="39" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="41" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="50" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="51" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="26" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="26" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="55" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="33" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="56" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="26" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="2" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="57" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1588,70 +1608,66 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="79" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="61" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="80" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="65" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="78" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="79" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="74" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="76" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="77" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="63" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="78" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="62" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="50" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="55" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="62" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="62" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="71" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="63" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="63" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="56" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="51" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2068,7 +2084,7 @@
   <dimension ref="A1:AA52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K49" sqref="K49"/>
+      <selection activeCell="A12" sqref="A12:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -2085,22 +2101,22 @@
   </cols>
   <sheetData>
     <row r="1" ht="23.25" customHeight="1">
-      <c r="A1" s="12" t="n"/>
-      <c r="B1" s="139" t="inlineStr">
+      <c r="A1" s="11" t="n"/>
+      <c r="B1" s="131" t="inlineStr">
         <is>
           <t>Registro da Qualidade</t>
         </is>
       </c>
-      <c r="C1" s="140" t="n"/>
-      <c r="D1" s="140" t="n"/>
-      <c r="E1" s="140" t="n"/>
-      <c r="F1" s="141" t="n"/>
-      <c r="G1" s="142" t="inlineStr">
+      <c r="C1" s="132" t="n"/>
+      <c r="D1" s="132" t="n"/>
+      <c r="E1" s="132" t="n"/>
+      <c r="F1" s="133" t="n"/>
+      <c r="G1" s="134" t="inlineStr">
         <is>
           <t>Código:</t>
         </is>
       </c>
-      <c r="H1" s="143" t="n"/>
+      <c r="H1" s="135" t="n"/>
       <c r="I1" s="1" t="inlineStr">
         <is>
           <t>RQ GQ-001-000</t>
@@ -2108,39 +2124,39 @@
       </c>
     </row>
     <row r="2" ht="23.25" customHeight="1">
-      <c r="A2" s="144" t="n"/>
-      <c r="B2" s="145" t="n"/>
-      <c r="C2" s="146" t="n"/>
-      <c r="D2" s="146" t="n"/>
-      <c r="E2" s="146" t="n"/>
-      <c r="F2" s="147" t="n"/>
-      <c r="G2" s="142" t="inlineStr">
+      <c r="A2" s="136" t="n"/>
+      <c r="B2" s="137" t="n"/>
+      <c r="C2" s="138" t="n"/>
+      <c r="D2" s="138" t="n"/>
+      <c r="E2" s="138" t="n"/>
+      <c r="F2" s="139" t="n"/>
+      <c r="G2" s="134" t="inlineStr">
         <is>
           <t>Data de Emissão:</t>
         </is>
       </c>
-      <c r="H2" s="143" t="n"/>
+      <c r="H2" s="135" t="n"/>
       <c r="I2" s="2" t="n">
         <v>45293</v>
       </c>
     </row>
     <row r="3" ht="23.25" customHeight="1">
-      <c r="A3" s="144" t="n"/>
-      <c r="B3" s="148" t="inlineStr">
+      <c r="A3" s="136" t="n"/>
+      <c r="B3" s="140" t="inlineStr">
         <is>
           <t>Gestão da Qualidade</t>
         </is>
       </c>
-      <c r="C3" s="140" t="n"/>
-      <c r="D3" s="140" t="n"/>
-      <c r="E3" s="140" t="n"/>
-      <c r="F3" s="141" t="n"/>
-      <c r="G3" s="142" t="inlineStr">
+      <c r="C3" s="132" t="n"/>
+      <c r="D3" s="132" t="n"/>
+      <c r="E3" s="132" t="n"/>
+      <c r="F3" s="133" t="n"/>
+      <c r="G3" s="134" t="inlineStr">
         <is>
           <t>Data da Última Revisão:</t>
         </is>
       </c>
-      <c r="H3" s="143" t="n"/>
+      <c r="H3" s="135" t="n"/>
       <c r="I3" s="3" t="inlineStr">
         <is>
           <t>-</t>
@@ -2148,74 +2164,74 @@
       </c>
     </row>
     <row r="4" ht="24" customHeight="1">
-      <c r="A4" s="144" t="n"/>
-      <c r="B4" s="149" t="n"/>
-      <c r="F4" s="150" t="n"/>
-      <c r="G4" s="151" t="inlineStr">
+      <c r="A4" s="136" t="n"/>
+      <c r="B4" s="141" t="n"/>
+      <c r="F4" s="142" t="n"/>
+      <c r="G4" s="143" t="inlineStr">
         <is>
           <t>Página:</t>
         </is>
       </c>
-      <c r="H4" s="141" t="n"/>
+      <c r="H4" s="133" t="n"/>
       <c r="I4" s="9" t="n">
         <v>44197</v>
       </c>
     </row>
     <row r="5" ht="24" customHeight="1">
-      <c r="A5" s="52" t="inlineStr">
+      <c r="A5" s="38" t="inlineStr">
         <is>
           <t>“Se você está lendo este documento em mídia impressa, esta é uma cópia Não-Controlada”</t>
         </is>
       </c>
-      <c r="B5" s="152" t="n"/>
-      <c r="C5" s="152" t="n"/>
-      <c r="D5" s="152" t="n"/>
-      <c r="E5" s="152" t="n"/>
-      <c r="F5" s="152" t="n"/>
-      <c r="G5" s="152" t="n"/>
-      <c r="H5" s="152" t="n"/>
-      <c r="I5" s="153" t="n"/>
+      <c r="B5" s="144" t="n"/>
+      <c r="C5" s="144" t="n"/>
+      <c r="D5" s="144" t="n"/>
+      <c r="E5" s="144" t="n"/>
+      <c r="F5" s="144" t="n"/>
+      <c r="G5" s="144" t="n"/>
+      <c r="H5" s="144" t="n"/>
+      <c r="I5" s="145" t="n"/>
     </row>
     <row r="6" ht="37.5" customHeight="1" thickBot="1">
-      <c r="A6" s="27" t="inlineStr">
+      <c r="A6" s="26" t="inlineStr">
         <is>
           <t>Relatório de Não Conformidade</t>
         </is>
       </c>
-      <c r="B6" s="152" t="n"/>
-      <c r="C6" s="152" t="n"/>
-      <c r="D6" s="152" t="n"/>
-      <c r="E6" s="152" t="n"/>
-      <c r="F6" s="152" t="n"/>
-      <c r="G6" s="152" t="n"/>
-      <c r="H6" s="152" t="n"/>
-      <c r="I6" s="153" t="n"/>
-    </row>
-    <row r="7" ht="24.75" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A7" s="29" t="inlineStr">
+      <c r="B6" s="144" t="n"/>
+      <c r="C6" s="144" t="n"/>
+      <c r="D6" s="144" t="n"/>
+      <c r="E6" s="144" t="n"/>
+      <c r="F6" s="144" t="n"/>
+      <c r="G6" s="144" t="n"/>
+      <c r="H6" s="144" t="n"/>
+      <c r="I6" s="145" t="n"/>
+    </row>
+    <row r="7" ht="24.75" customHeight="1" thickTop="1">
+      <c r="A7" s="28" t="inlineStr">
         <is>
           <t>1ª ETAPA - ABERTURA</t>
         </is>
       </c>
-      <c r="B7" s="154" t="n"/>
-      <c r="C7" s="154" t="n"/>
-      <c r="D7" s="154" t="n"/>
-      <c r="E7" s="154" t="n"/>
-      <c r="F7" s="11" t="inlineStr">
+      <c r="B7" s="146" t="n"/>
+      <c r="C7" s="146" t="n"/>
+      <c r="D7" s="146" t="n"/>
+      <c r="E7" s="146" t="n"/>
+      <c r="F7" s="10" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="G7" s="32" t="inlineStr">
-        <is>
-          <t>Feito</t>
-        </is>
-      </c>
-      <c r="H7" s="155" t="n"/>
-      <c r="I7" s="156" t="n"/>
+      <c r="G7" s="46" t="inlineStr">
+        <is>
+          <t>Verificação</t>
+        </is>
+      </c>
+      <c r="H7" s="147" t="n"/>
+      <c r="I7" s="148" t="n"/>
       <c r="J7" s="4" t="n"/>
       <c r="K7" s="4" t="n"/>
-      <c r="L7" s="24" t="n"/>
+      <c r="L7" s="23" t="n"/>
       <c r="M7" s="4" t="n"/>
       <c r="N7" s="4" t="n"/>
       <c r="O7" s="4" t="n"/>
@@ -2233,207 +2249,217 @@
       <c r="AA7" s="4" t="n"/>
     </row>
     <row r="8" ht="22.5" customHeight="1">
-      <c r="A8" s="57" t="inlineStr">
+      <c r="A8" s="128" t="inlineStr">
         <is>
           <t>RNC Nº</t>
         </is>
       </c>
-      <c r="B8" s="59" t="n">
-        <v>5744182532</v>
-      </c>
-      <c r="C8" s="95" t="inlineStr">
+      <c r="B8" s="47" t="n">
+        <v>5832164054</v>
+      </c>
+      <c r="C8" s="129" t="inlineStr">
         <is>
           <t>Origem:</t>
         </is>
       </c>
-      <c r="D8" s="59" t="inlineStr">
-        <is>
-          <t>Direção</t>
-        </is>
-      </c>
-      <c r="E8" s="157" t="n"/>
-      <c r="F8" s="97" t="inlineStr">
+      <c r="D8" s="47" t="inlineStr">
+        <is>
+          <t>Gestão da Qualidade</t>
+        </is>
+      </c>
+      <c r="E8" s="149" t="n"/>
+      <c r="F8" s="130" t="inlineStr">
         <is>
           <t>Resp.:</t>
         </is>
       </c>
-      <c r="G8" s="61" t="inlineStr">
+      <c r="G8" s="44" t="inlineStr">
         <is>
           <t>Amanda Prado</t>
         </is>
       </c>
-      <c r="H8" s="97" t="inlineStr">
+      <c r="H8" s="130" t="inlineStr">
         <is>
           <t>Data:</t>
         </is>
       </c>
-      <c r="I8" s="64" t="inlineStr">
-        <is>
-          <t>31/01/2024</t>
-        </is>
-      </c>
-      <c r="L8" s="24" t="n"/>
+      <c r="I8" s="44" t="inlineStr">
+        <is>
+          <t>03/01/2024</t>
+        </is>
+      </c>
+      <c r="L8" s="23" t="n"/>
     </row>
     <row r="9" ht="41.25" customHeight="1">
-      <c r="A9" s="158" t="n"/>
-      <c r="F9" s="97" t="inlineStr">
+      <c r="A9" s="150" t="n"/>
+      <c r="B9" s="150" t="n"/>
+      <c r="C9" s="150" t="n"/>
+      <c r="D9" s="151" t="n"/>
+      <c r="E9" s="152" t="n"/>
+      <c r="F9" s="130" t="inlineStr">
         <is>
           <t>Item Norma:</t>
         </is>
       </c>
-      <c r="G9" s="64" t="inlineStr">
-        <is>
-          <t>5.1.2</t>
-        </is>
-      </c>
-      <c r="I9" s="159" t="n"/>
+      <c r="G9" s="44" t="inlineStr">
+        <is>
+          <t>9.2.2</t>
+        </is>
+      </c>
+      <c r="H9" s="144" t="n"/>
+      <c r="I9" s="145" t="n"/>
     </row>
     <row r="10" ht="22.5" customHeight="1">
-      <c r="A10" s="160" t="n"/>
-      <c r="I10" s="159" t="n"/>
+      <c r="A10" s="30" t="n"/>
+      <c r="B10" s="144" t="n"/>
+      <c r="C10" s="144" t="n"/>
+      <c r="D10" s="144" t="n"/>
+      <c r="E10" s="144" t="n"/>
+      <c r="F10" s="144" t="n"/>
+      <c r="G10" s="144" t="n"/>
+      <c r="H10" s="144" t="n"/>
+      <c r="I10" s="145" t="n"/>
     </row>
     <row r="11" ht="24.95" customFormat="1" customHeight="1" s="6">
-      <c r="A11" s="99" t="inlineStr">
+      <c r="A11" s="130" t="inlineStr">
         <is>
           <t>Descrição do Problema</t>
         </is>
       </c>
-      <c r="F11" s="99" t="inlineStr">
+      <c r="B11" s="144" t="n"/>
+      <c r="C11" s="144" t="n"/>
+      <c r="D11" s="144" t="n"/>
+      <c r="E11" s="145" t="n"/>
+      <c r="F11" s="130" t="inlineStr">
         <is>
           <t>Conj / Ativ:</t>
         </is>
       </c>
-      <c r="G11" s="64" t="inlineStr">
+      <c r="G11" s="44" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="I11" s="159" t="n"/>
-    </row>
-    <row r="12" ht="66.75" customFormat="1" customHeight="1" s="6" thickBot="1">
-      <c r="A12" s="161" t="inlineStr">
-        <is>
-          <t>Não há um compromisso de satisfazer os requisitos aplicáveis na Política da Qualidade</t>
-        </is>
-      </c>
-      <c r="B12" s="162" t="n"/>
-      <c r="C12" s="162" t="n"/>
-      <c r="D12" s="162" t="n"/>
-      <c r="E12" s="162" t="n"/>
-      <c r="F12" s="162" t="n"/>
-      <c r="G12" s="162" t="n"/>
-      <c r="H12" s="162" t="n"/>
-      <c r="I12" s="163" t="n"/>
+      <c r="H11" s="144" t="n"/>
+      <c r="I11" s="145" t="n"/>
+    </row>
+    <row r="12" ht="66.75" customFormat="1" customHeight="1" s="6">
+      <c r="A12" s="48" t="inlineStr">
+        <is>
+          <t>NC 36: Não há o relatório de auditoria interna - RQ GQ-011-002 do mês de abril de 2023.</t>
+        </is>
+      </c>
+      <c r="B12" s="144" t="n"/>
+      <c r="C12" s="144" t="n"/>
+      <c r="D12" s="144" t="n"/>
+      <c r="E12" s="144" t="n"/>
+      <c r="F12" s="144" t="n"/>
+      <c r="G12" s="144" t="n"/>
+      <c r="H12" s="144" t="n"/>
+      <c r="I12" s="145" t="n"/>
     </row>
     <row r="13" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A13" s="164" t="n"/>
-      <c r="B13" s="140" t="n"/>
-      <c r="C13" s="140" t="n"/>
-      <c r="D13" s="140" t="n"/>
-      <c r="E13" s="140" t="n"/>
-      <c r="F13" s="140" t="n"/>
-      <c r="G13" s="140" t="n"/>
-      <c r="H13" s="140" t="n"/>
-      <c r="I13" s="165" t="n"/>
+      <c r="A13" s="153" t="n"/>
+      <c r="I13" s="154" t="n"/>
     </row>
     <row r="14" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A14" s="166" t="inlineStr">
+      <c r="A14" s="155" t="inlineStr">
         <is>
           <t>2ª ETAPA - AÇÃO IMEDIATA</t>
         </is>
       </c>
-      <c r="B14" s="167" t="n"/>
-      <c r="C14" s="167" t="n"/>
-      <c r="D14" s="167" t="n"/>
-      <c r="E14" s="168" t="n"/>
-      <c r="F14" s="107" t="inlineStr">
+      <c r="B14" s="147" t="n"/>
+      <c r="C14" s="147" t="n"/>
+      <c r="D14" s="147" t="n"/>
+      <c r="E14" s="156" t="n"/>
+      <c r="F14" s="119" t="inlineStr">
         <is>
           <t>Status:</t>
         </is>
       </c>
-      <c r="G14" s="70" t="inlineStr">
+      <c r="G14" s="60" t="inlineStr">
         <is>
           <t>Feito</t>
         </is>
       </c>
-      <c r="H14" s="107" t="inlineStr">
+      <c r="H14" s="119" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
       </c>
-      <c r="I14" s="70" t="inlineStr">
-        <is>
-          <t>05/01/2024</t>
+      <c r="I14" s="60" t="inlineStr">
+        <is>
+          <t>20/01/2024</t>
         </is>
       </c>
     </row>
     <row r="15" ht="48" customHeight="1" thickBot="1">
-      <c r="A15" s="169" t="n"/>
-      <c r="B15" s="162" t="n"/>
-      <c r="C15" s="162" t="n"/>
-      <c r="D15" s="162" t="n"/>
-      <c r="E15" s="163" t="n"/>
-      <c r="F15" s="106" t="inlineStr">
+      <c r="A15" s="157" t="n"/>
+      <c r="B15" s="158" t="n"/>
+      <c r="C15" s="158" t="n"/>
+      <c r="D15" s="158" t="n"/>
+      <c r="E15" s="159" t="n"/>
+      <c r="F15" s="118" t="inlineStr">
         <is>
           <t>Resp.:</t>
         </is>
       </c>
-      <c r="G15" s="69" t="inlineStr">
+      <c r="G15" s="59" t="inlineStr">
         <is>
           <t>Amanda Prado</t>
         </is>
       </c>
-      <c r="H15" s="170" t="n"/>
-      <c r="I15" s="171" t="n"/>
+      <c r="H15" s="160" t="n"/>
+      <c r="I15" s="161" t="n"/>
     </row>
     <row r="16" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A16" s="108" t="inlineStr">
+      <c r="A16" s="124" t="inlineStr">
         <is>
           <t>Ação imediata</t>
         </is>
       </c>
-      <c r="B16" s="140" t="n"/>
-      <c r="C16" s="140" t="n"/>
-      <c r="D16" s="140" t="n"/>
-      <c r="E16" s="140" t="n"/>
-      <c r="F16" s="140" t="n"/>
-      <c r="G16" s="140" t="n"/>
-      <c r="H16" s="140" t="n"/>
-      <c r="I16" s="141" t="n"/>
+      <c r="B16" s="132" t="n"/>
+      <c r="C16" s="132" t="n"/>
+      <c r="D16" s="132" t="n"/>
+      <c r="E16" s="132" t="n"/>
+      <c r="F16" s="132" t="n"/>
+      <c r="G16" s="132" t="n"/>
+      <c r="H16" s="132" t="n"/>
+      <c r="I16" s="133" t="n"/>
     </row>
     <row r="17" ht="27.95" customFormat="1" customHeight="1" s="6">
-      <c r="A17" s="71" t="inlineStr">
-        <is>
-          <t>Alteração na Política da Qualidade</t>
-        </is>
-      </c>
-      <c r="B17" s="167" t="n"/>
-      <c r="C17" s="167" t="n"/>
-      <c r="D17" s="167" t="n"/>
-      <c r="E17" s="167" t="n"/>
-      <c r="F17" s="167" t="n"/>
-      <c r="G17" s="167" t="n"/>
-      <c r="H17" s="167" t="n"/>
-      <c r="I17" s="172" t="n"/>
+      <c r="A17" s="49" t="inlineStr">
+        <is>
+          <t>Preenchimento do relatório de auditoria pendente</t>
+        </is>
+      </c>
+      <c r="B17" s="147" t="n"/>
+      <c r="C17" s="147" t="n"/>
+      <c r="D17" s="147" t="n"/>
+      <c r="E17" s="147" t="n"/>
+      <c r="F17" s="147" t="n"/>
+      <c r="G17" s="147" t="n"/>
+      <c r="H17" s="147" t="n"/>
+      <c r="I17" s="162" t="n"/>
     </row>
     <row r="18" ht="27.95" customFormat="1" customHeight="1" s="6">
-      <c r="A18" s="173" t="n"/>
-      <c r="I18" s="150" t="n"/>
+      <c r="A18" s="163" t="n"/>
+      <c r="I18" s="142" t="n"/>
     </row>
     <row r="19" ht="27.95" customFormat="1" customHeight="1" s="6">
-      <c r="A19" s="173" t="n"/>
-      <c r="I19" s="150" t="n"/>
+      <c r="A19" s="163" t="n"/>
+      <c r="I19" s="142" t="n"/>
     </row>
     <row r="20" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A20" s="174" t="n"/>
-      <c r="B20" s="146" t="n"/>
-      <c r="C20" s="146" t="n"/>
-      <c r="D20" s="146" t="n"/>
-      <c r="E20" s="146" t="n"/>
-      <c r="F20" s="146" t="n"/>
-      <c r="G20" s="146" t="n"/>
-      <c r="H20" s="146" t="n"/>
-      <c r="I20" s="147" t="n"/>
+      <c r="A20" s="164" t="n"/>
+      <c r="B20" s="138" t="n"/>
+      <c r="C20" s="138" t="n"/>
+      <c r="D20" s="138" t="n"/>
+      <c r="E20" s="138" t="n"/>
+      <c r="F20" s="138" t="n"/>
+      <c r="G20" s="138" t="n"/>
+      <c r="H20" s="138" t="n"/>
+      <c r="I20" s="139" t="n"/>
       <c r="J20" s="4" t="n"/>
       <c r="K20" s="4" t="n"/>
       <c r="L20" s="4" t="n"/>
@@ -2454,216 +2480,214 @@
       <c r="AA20" s="4" t="n"/>
     </row>
     <row r="21" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A21" s="39" t="n"/>
-      <c r="B21" s="175" t="n"/>
-      <c r="C21" s="175" t="n"/>
-      <c r="D21" s="175" t="n"/>
-      <c r="E21" s="175" t="n"/>
-      <c r="F21" s="175" t="n"/>
-      <c r="G21" s="175" t="n"/>
-      <c r="H21" s="175" t="n"/>
-      <c r="I21" s="176" t="n"/>
+      <c r="A21" s="34" t="n"/>
+      <c r="B21" s="165" t="n"/>
+      <c r="C21" s="165" t="n"/>
+      <c r="D21" s="165" t="n"/>
+      <c r="E21" s="165" t="n"/>
+      <c r="F21" s="165" t="n"/>
+      <c r="G21" s="165" t="n"/>
+      <c r="H21" s="165" t="n"/>
+      <c r="I21" s="166" t="n"/>
     </row>
     <row r="22" ht="18.75" customHeight="1">
-      <c r="A22" s="177" t="inlineStr">
+      <c r="A22" s="167" t="inlineStr">
         <is>
           <t>3ª ETAPA - ANÁLISE DE CAUZA RAIZ</t>
         </is>
       </c>
-      <c r="B22" s="157" t="n"/>
-      <c r="C22" s="157" t="n"/>
-      <c r="D22" s="157" t="n"/>
-      <c r="E22" s="178" t="n"/>
-      <c r="F22" s="179" t="inlineStr">
+      <c r="B22" s="168" t="n"/>
+      <c r="C22" s="168" t="n"/>
+      <c r="D22" s="168" t="n"/>
+      <c r="E22" s="169" t="n"/>
+      <c r="F22" s="170" t="inlineStr">
         <is>
           <t>Resp.:</t>
         </is>
       </c>
-      <c r="G22" s="86" t="inlineStr">
+      <c r="G22" s="76" t="inlineStr">
         <is>
           <t>Amanda Prado</t>
         </is>
       </c>
-      <c r="H22" s="179" t="inlineStr">
+      <c r="H22" s="170" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
       </c>
-      <c r="I22" s="86" t="inlineStr">
-        <is>
-          <t>08/01/2024</t>
-        </is>
+      <c r="I22" s="76" t="n">
+        <v/>
       </c>
     </row>
     <row r="23" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A23" s="180" t="n"/>
-      <c r="B23" s="162" t="n"/>
-      <c r="C23" s="162" t="n"/>
-      <c r="D23" s="162" t="n"/>
-      <c r="E23" s="163" t="n"/>
-      <c r="F23" s="180" t="n"/>
-      <c r="G23" s="163" t="n"/>
-      <c r="H23" s="180" t="n"/>
-      <c r="I23" s="163" t="n"/>
+      <c r="A23" s="171" t="n"/>
+      <c r="B23" s="158" t="n"/>
+      <c r="C23" s="158" t="n"/>
+      <c r="D23" s="158" t="n"/>
+      <c r="E23" s="159" t="n"/>
+      <c r="F23" s="171" t="n"/>
+      <c r="G23" s="159" t="n"/>
+      <c r="H23" s="171" t="n"/>
+      <c r="I23" s="159" t="n"/>
     </row>
     <row r="24" ht="45" customHeight="1">
-      <c r="A24" s="117" t="inlineStr">
+      <c r="A24" s="112" t="inlineStr">
         <is>
           <t>Máquina</t>
         </is>
       </c>
-      <c r="B24" s="181" t="inlineStr">
+      <c r="B24" s="172" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="C24" s="140" t="n"/>
-      <c r="D24" s="140" t="n"/>
-      <c r="E24" s="140" t="n"/>
-      <c r="F24" s="140" t="n"/>
-      <c r="G24" s="140" t="n"/>
-      <c r="H24" s="140" t="n"/>
-      <c r="I24" s="141" t="n"/>
+      <c r="C24" s="132" t="n"/>
+      <c r="D24" s="132" t="n"/>
+      <c r="E24" s="132" t="n"/>
+      <c r="F24" s="132" t="n"/>
+      <c r="G24" s="132" t="n"/>
+      <c r="H24" s="132" t="n"/>
+      <c r="I24" s="133" t="n"/>
     </row>
     <row r="25" ht="45" customHeight="1">
-      <c r="A25" s="117" t="inlineStr">
+      <c r="A25" s="112" t="inlineStr">
         <is>
           <t>Mão-de-Obra</t>
         </is>
       </c>
-      <c r="B25" s="46" t="inlineStr">
+      <c r="B25" s="67" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="C25" s="182" t="n"/>
-      <c r="D25" s="182" t="n"/>
-      <c r="E25" s="182" t="n"/>
-      <c r="F25" s="182" t="n"/>
-      <c r="G25" s="182" t="n"/>
-      <c r="H25" s="182" t="n"/>
-      <c r="I25" s="183" t="n"/>
+      <c r="C25" s="173" t="n"/>
+      <c r="D25" s="173" t="n"/>
+      <c r="E25" s="173" t="n"/>
+      <c r="F25" s="173" t="n"/>
+      <c r="G25" s="173" t="n"/>
+      <c r="H25" s="173" t="n"/>
+      <c r="I25" s="174" t="n"/>
     </row>
     <row r="26" ht="45" customHeight="1">
-      <c r="A26" s="117" t="inlineStr">
+      <c r="A26" s="112" t="inlineStr">
         <is>
           <t>Matéria Prima</t>
         </is>
       </c>
-      <c r="B26" s="46" t="inlineStr">
+      <c r="B26" s="67" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="C26" s="182" t="n"/>
-      <c r="D26" s="182" t="n"/>
-      <c r="E26" s="182" t="n"/>
-      <c r="F26" s="182" t="n"/>
-      <c r="G26" s="182" t="n"/>
-      <c r="H26" s="182" t="n"/>
-      <c r="I26" s="183" t="n"/>
+      <c r="C26" s="173" t="n"/>
+      <c r="D26" s="173" t="n"/>
+      <c r="E26" s="173" t="n"/>
+      <c r="F26" s="173" t="n"/>
+      <c r="G26" s="173" t="n"/>
+      <c r="H26" s="173" t="n"/>
+      <c r="I26" s="174" t="n"/>
     </row>
     <row r="27" ht="45" customHeight="1">
-      <c r="A27" s="117" t="inlineStr">
+      <c r="A27" s="112" t="inlineStr">
         <is>
           <t>Medição</t>
         </is>
       </c>
-      <c r="B27" s="46" t="inlineStr">
+      <c r="B27" s="67" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="C27" s="182" t="n"/>
-      <c r="D27" s="182" t="n"/>
-      <c r="E27" s="182" t="n"/>
-      <c r="F27" s="182" t="n"/>
-      <c r="G27" s="182" t="n"/>
-      <c r="H27" s="182" t="n"/>
-      <c r="I27" s="183" t="n"/>
+      <c r="C27" s="173" t="n"/>
+      <c r="D27" s="173" t="n"/>
+      <c r="E27" s="173" t="n"/>
+      <c r="F27" s="173" t="n"/>
+      <c r="G27" s="173" t="n"/>
+      <c r="H27" s="173" t="n"/>
+      <c r="I27" s="174" t="n"/>
     </row>
     <row r="28" ht="45" customHeight="1">
-      <c r="A28" s="117" t="inlineStr">
+      <c r="A28" s="112" t="inlineStr">
         <is>
           <t>Método</t>
         </is>
       </c>
-      <c r="B28" s="46" t="inlineStr">
-        <is>
-          <t>Não havia conhecimento sobre a necessidade em questão</t>
-        </is>
-      </c>
-      <c r="C28" s="182" t="n"/>
-      <c r="D28" s="182" t="n"/>
-      <c r="E28" s="182" t="n"/>
-      <c r="F28" s="182" t="n"/>
-      <c r="G28" s="182" t="n"/>
-      <c r="H28" s="182" t="n"/>
-      <c r="I28" s="183" t="n"/>
+      <c r="B28" s="67" t="inlineStr">
+        <is>
+          <t>Não havia definição documentada</t>
+        </is>
+      </c>
+      <c r="C28" s="173" t="n"/>
+      <c r="D28" s="173" t="n"/>
+      <c r="E28" s="173" t="n"/>
+      <c r="F28" s="173" t="n"/>
+      <c r="G28" s="173" t="n"/>
+      <c r="H28" s="173" t="n"/>
+      <c r="I28" s="174" t="n"/>
     </row>
     <row r="29" ht="45" customHeight="1">
-      <c r="A29" s="117" t="inlineStr">
+      <c r="A29" s="112" t="inlineStr">
         <is>
           <t>Meio Ambiente</t>
         </is>
       </c>
-      <c r="B29" s="46" t="inlineStr">
+      <c r="B29" s="67" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="C29" s="182" t="n"/>
-      <c r="D29" s="182" t="n"/>
-      <c r="E29" s="182" t="n"/>
-      <c r="F29" s="182" t="n"/>
-      <c r="G29" s="182" t="n"/>
-      <c r="H29" s="182" t="n"/>
-      <c r="I29" s="183" t="n"/>
+      <c r="C29" s="173" t="n"/>
+      <c r="D29" s="173" t="n"/>
+      <c r="E29" s="173" t="n"/>
+      <c r="F29" s="173" t="n"/>
+      <c r="G29" s="173" t="n"/>
+      <c r="H29" s="173" t="n"/>
+      <c r="I29" s="174" t="n"/>
     </row>
     <row r="30" ht="45" customHeight="1">
-      <c r="A30" s="118" t="inlineStr">
+      <c r="A30" s="110" t="inlineStr">
         <is>
           <t>Presentes:</t>
         </is>
       </c>
-      <c r="B30" s="184" t="n"/>
-      <c r="C30" s="48" t="inlineStr">
+      <c r="B30" s="175" t="n"/>
+      <c r="C30" s="69" t="inlineStr">
         <is>
           <t>Amanda</t>
         </is>
       </c>
-      <c r="D30" s="185" t="n"/>
-      <c r="E30" s="185" t="n"/>
-      <c r="F30" s="185" t="n"/>
-      <c r="G30" s="185" t="n"/>
-      <c r="H30" s="185" t="n"/>
-      <c r="I30" s="184" t="n"/>
+      <c r="D30" s="176" t="n"/>
+      <c r="E30" s="176" t="n"/>
+      <c r="F30" s="176" t="n"/>
+      <c r="G30" s="176" t="n"/>
+      <c r="H30" s="176" t="n"/>
+      <c r="I30" s="175" t="n"/>
     </row>
     <row r="31" ht="6" customHeight="1" thickBot="1">
-      <c r="A31" s="51" t="n"/>
-      <c r="B31" s="186" t="n"/>
-      <c r="C31" s="186" t="n"/>
-      <c r="D31" s="186" t="n"/>
-      <c r="E31" s="186" t="n"/>
-      <c r="F31" s="186" t="n"/>
-      <c r="G31" s="186" t="n"/>
-      <c r="H31" s="186" t="n"/>
-      <c r="I31" s="187" t="n"/>
+      <c r="A31" s="37" t="n"/>
+      <c r="B31" s="177" t="n"/>
+      <c r="C31" s="177" t="n"/>
+      <c r="D31" s="177" t="n"/>
+      <c r="E31" s="177" t="n"/>
+      <c r="F31" s="177" t="n"/>
+      <c r="G31" s="177" t="n"/>
+      <c r="H31" s="177" t="n"/>
+      <c r="I31" s="178" t="n"/>
     </row>
     <row r="32" ht="36.75" customHeight="1" thickBot="1">
-      <c r="A32" s="177" t="inlineStr">
+      <c r="A32" s="167" t="inlineStr">
         <is>
           <t>3ªETAPA - PLANO DE AÇÃO</t>
         </is>
       </c>
-      <c r="B32" s="170" t="n"/>
-      <c r="C32" s="170" t="n"/>
-      <c r="D32" s="170" t="n"/>
-      <c r="E32" s="170" t="n"/>
-      <c r="F32" s="170" t="n"/>
-      <c r="G32" s="170" t="n"/>
-      <c r="H32" s="170" t="n"/>
-      <c r="I32" s="188" t="n"/>
+      <c r="B32" s="160" t="n"/>
+      <c r="C32" s="160" t="n"/>
+      <c r="D32" s="160" t="n"/>
+      <c r="E32" s="160" t="n"/>
+      <c r="F32" s="160" t="n"/>
+      <c r="G32" s="160" t="n"/>
+      <c r="H32" s="160" t="n"/>
+      <c r="I32" s="179" t="n"/>
       <c r="J32" s="4" t="n"/>
       <c r="K32" s="4" t="n"/>
       <c r="L32" s="4" t="n"/>
@@ -2684,235 +2708,275 @@
       <c r="AA32" s="4" t="n"/>
     </row>
     <row r="33" ht="18.75" customHeight="1">
-      <c r="A33" s="189" t="inlineStr">
+      <c r="A33" s="180" t="inlineStr">
         <is>
           <t>Atividade</t>
         </is>
       </c>
-      <c r="B33" s="157" t="n"/>
-      <c r="C33" s="157" t="n"/>
-      <c r="D33" s="178" t="n"/>
-      <c r="E33" s="189" t="inlineStr">
+      <c r="B33" s="168" t="n"/>
+      <c r="C33" s="168" t="n"/>
+      <c r="D33" s="169" t="n"/>
+      <c r="E33" s="180" t="inlineStr">
         <is>
           <t>Responsável</t>
         </is>
       </c>
-      <c r="F33" s="189" t="inlineStr">
+      <c r="F33" s="180" t="inlineStr">
         <is>
           <t>Previsão</t>
         </is>
       </c>
-      <c r="G33" s="178" t="n"/>
-      <c r="H33" s="189" t="inlineStr">
+      <c r="G33" s="169" t="n"/>
+      <c r="H33" s="180" t="inlineStr">
         <is>
           <t>Realizado</t>
         </is>
       </c>
-      <c r="I33" s="178" t="n"/>
+      <c r="I33" s="169" t="n"/>
     </row>
     <row r="34" ht="9" customHeight="1" thickBot="1">
-      <c r="A34" s="180" t="n"/>
-      <c r="B34" s="162" t="n"/>
-      <c r="C34" s="162" t="n"/>
-      <c r="D34" s="163" t="n"/>
-      <c r="E34" s="190" t="n"/>
-      <c r="F34" s="180" t="n"/>
-      <c r="G34" s="163" t="n"/>
-      <c r="H34" s="180" t="n"/>
-      <c r="I34" s="163" t="n"/>
+      <c r="A34" s="171" t="n"/>
+      <c r="B34" s="158" t="n"/>
+      <c r="C34" s="158" t="n"/>
+      <c r="D34" s="159" t="n"/>
+      <c r="E34" s="181" t="n"/>
+      <c r="F34" s="171" t="n"/>
+      <c r="G34" s="159" t="n"/>
+      <c r="H34" s="171" t="n"/>
+      <c r="I34" s="159" t="n"/>
     </row>
     <row r="35" ht="60" customFormat="1" customHeight="1" s="6" thickBot="1">
-      <c r="A35" s="191" t="inlineStr">
-        <is>
-          <t>Criação do Manual da Qualidade CEMAG</t>
-        </is>
-      </c>
-      <c r="B35" s="170" t="n"/>
-      <c r="C35" s="170" t="n"/>
-      <c r="D35" s="188" t="n"/>
-      <c r="E35" s="85" t="inlineStr">
+      <c r="A35" s="182" t="inlineStr">
+        <is>
+          <t>Determinar frequência mais adequada para a realização de auditorias internas (copy) (copy)</t>
+        </is>
+      </c>
+      <c r="B35" s="160" t="n"/>
+      <c r="C35" s="160" t="n"/>
+      <c r="D35" s="179" t="n"/>
+      <c r="E35" s="75" t="inlineStr">
         <is>
           <t>Amanda Prado</t>
         </is>
       </c>
-      <c r="F35" s="191" t="inlineStr">
-        <is>
-          <t>05/01/2024</t>
-        </is>
-      </c>
-      <c r="G35" s="188" t="n"/>
-      <c r="H35" s="191" t="inlineStr">
-        <is>
-          <t>05/01/2024</t>
-        </is>
-      </c>
-      <c r="I35" s="188" t="n"/>
+      <c r="F35" s="182" t="inlineStr">
+        <is>
+          <t>04/01/2024</t>
+        </is>
+      </c>
+      <c r="G35" s="179" t="n"/>
+      <c r="H35" s="182" t="inlineStr">
+        <is>
+          <t>04/01/2024</t>
+        </is>
+      </c>
+      <c r="I35" s="179" t="n"/>
     </row>
     <row r="36" ht="60" customFormat="1" customHeight="1" s="6" thickBot="1">
-      <c r="A36" s="191" t="n">
+      <c r="A36" s="182" t="inlineStr">
+        <is>
+          <t>Criar Procedimento de Auditorias Internas (copy) (copy)</t>
+        </is>
+      </c>
+      <c r="B36" s="160" t="n"/>
+      <c r="C36" s="160" t="n"/>
+      <c r="D36" s="179" t="n"/>
+      <c r="E36" s="75" t="inlineStr">
+        <is>
+          <t>Amanda Prado</t>
+        </is>
+      </c>
+      <c r="F36" s="182" t="inlineStr">
+        <is>
+          <t>04/01/2024</t>
+        </is>
+      </c>
+      <c r="G36" s="179" t="n"/>
+      <c r="H36" s="182" t="inlineStr">
+        <is>
+          <t>04/01/2024</t>
+        </is>
+      </c>
+      <c r="I36" s="179" t="n"/>
+    </row>
+    <row r="37" ht="60" customFormat="1" customHeight="1" s="6" thickBot="1">
+      <c r="A37" s="182" t="inlineStr">
+        <is>
+          <t>Criar Programa de Auditorias Internas de 2024 (copy) (copy)</t>
+        </is>
+      </c>
+      <c r="B37" s="160" t="n"/>
+      <c r="C37" s="160" t="n"/>
+      <c r="D37" s="179" t="n"/>
+      <c r="E37" s="75" t="inlineStr">
+        <is>
+          <t>Amanda Prado</t>
+        </is>
+      </c>
+      <c r="F37" s="182" t="inlineStr">
+        <is>
+          <t>11/01/2024</t>
+        </is>
+      </c>
+      <c r="G37" s="179" t="n"/>
+      <c r="H37" s="182" t="inlineStr">
+        <is>
+          <t>08/01/2024</t>
+        </is>
+      </c>
+      <c r="I37" s="179" t="n"/>
+    </row>
+    <row r="38" ht="60" customFormat="1" customHeight="1" s="6" thickBot="1">
+      <c r="A38" s="182" t="inlineStr">
+        <is>
+          <t>Divulgar Procedimento (copy) (copy)</t>
+        </is>
+      </c>
+      <c r="B38" s="160" t="n"/>
+      <c r="C38" s="160" t="n"/>
+      <c r="D38" s="179" t="n"/>
+      <c r="E38" s="75" t="inlineStr">
+        <is>
+          <t>Amanda Prado</t>
+        </is>
+      </c>
+      <c r="F38" s="182" t="inlineStr">
+        <is>
+          <t>31/01/2024</t>
+        </is>
+      </c>
+      <c r="G38" s="179" t="n"/>
+      <c r="H38" s="182" t="n"/>
+      <c r="I38" s="179" t="n"/>
+    </row>
+    <row r="39" ht="60" customFormat="1" customHeight="1" s="6" thickBot="1">
+      <c r="A39" s="182" t="n"/>
+      <c r="B39" s="160" t="n"/>
+      <c r="C39" s="160" t="n"/>
+      <c r="D39" s="179" t="n"/>
+      <c r="E39" s="75" t="n"/>
+      <c r="F39" s="182" t="n"/>
+      <c r="G39" s="179" t="n"/>
+      <c r="H39" s="182" t="n"/>
+      <c r="I39" s="179" t="n"/>
+    </row>
+    <row r="40" ht="60" customFormat="1" customHeight="1" s="6" thickBot="1">
+      <c r="A40" s="182" t="n"/>
+      <c r="B40" s="160" t="n"/>
+      <c r="C40" s="160" t="n"/>
+      <c r="D40" s="179" t="n"/>
+      <c r="E40" s="75" t="n"/>
+      <c r="F40" s="182" t="n"/>
+      <c r="G40" s="179" t="n"/>
+      <c r="H40" s="182" t="n"/>
+      <c r="I40" s="179" t="n"/>
+    </row>
+    <row r="41" ht="60" customFormat="1" customHeight="1" s="6" thickBot="1">
+      <c r="A41" s="182" t="n"/>
+      <c r="B41" s="160" t="n"/>
+      <c r="C41" s="160" t="n"/>
+      <c r="D41" s="179" t="n"/>
+      <c r="E41" s="75" t="n"/>
+      <c r="F41" s="182" t="n"/>
+      <c r="G41" s="179" t="n"/>
+      <c r="H41" s="182" t="n"/>
+      <c r="I41" s="179" t="n"/>
+    </row>
+    <row r="42" ht="60" customFormat="1" customHeight="1" s="6" thickBot="1">
+      <c r="A42" s="182" t="n"/>
+      <c r="B42" s="160" t="n"/>
+      <c r="C42" s="160" t="n"/>
+      <c r="D42" s="179" t="n"/>
+      <c r="E42" s="75" t="n"/>
+      <c r="F42" s="182" t="n"/>
+      <c r="G42" s="179" t="n"/>
+      <c r="H42" s="182" t="n"/>
+      <c r="I42" s="179" t="n"/>
+    </row>
+    <row r="43" ht="60" customFormat="1" customHeight="1" s="6" thickBot="1">
+      <c r="A43" s="182" t="n"/>
+      <c r="B43" s="160" t="n"/>
+      <c r="C43" s="160" t="n"/>
+      <c r="D43" s="179" t="n"/>
+      <c r="E43" s="75" t="n"/>
+      <c r="F43" s="182" t="n"/>
+      <c r="G43" s="179" t="n"/>
+      <c r="H43" s="182" t="n"/>
+      <c r="I43" s="179" t="n"/>
+    </row>
+    <row r="44" ht="60" customFormat="1" customHeight="1" s="6" thickBot="1">
+      <c r="A44" s="182" t="n"/>
+      <c r="B44" s="160" t="n"/>
+      <c r="C44" s="160" t="n"/>
+      <c r="D44" s="179" t="n"/>
+      <c r="E44" s="75" t="n"/>
+      <c r="F44" s="182" t="n"/>
+      <c r="G44" s="179" t="n"/>
+      <c r="H44" s="182" t="n"/>
+      <c r="I44" s="179" t="n"/>
+    </row>
+    <row r="45" ht="6" customHeight="1" thickBot="1">
+      <c r="A45" s="40" t="n"/>
+      <c r="B45" s="176" t="n"/>
+      <c r="C45" s="176" t="n"/>
+      <c r="D45" s="176" t="n"/>
+      <c r="E45" s="176" t="n"/>
+      <c r="F45" s="176" t="n"/>
+      <c r="G45" s="176" t="n"/>
+      <c r="H45" s="176" t="n"/>
+      <c r="I45" s="175" t="n"/>
+    </row>
+    <row r="46" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A46" s="183" t="inlineStr">
+        <is>
+          <t>4ª ETAPA - EFICÁCIA</t>
+        </is>
+      </c>
+      <c r="B46" s="168" t="n"/>
+      <c r="C46" s="168" t="n"/>
+      <c r="D46" s="168" t="n"/>
+      <c r="E46" s="169" t="n"/>
+      <c r="F46" s="98" t="inlineStr">
+        <is>
+          <t>Data</t>
+        </is>
+      </c>
+      <c r="G46" s="76" t="inlineStr">
+        <is>
+          <t>11/01/2024</t>
+        </is>
+      </c>
+      <c r="H46" s="160" t="n"/>
+      <c r="I46" s="179" t="n"/>
+    </row>
+    <row r="47" ht="18.75" customHeight="1">
+      <c r="A47" s="184" t="n"/>
+      <c r="E47" s="185" t="n"/>
+      <c r="F47" s="97" t="inlineStr">
+        <is>
+          <t>Resp.:</t>
+        </is>
+      </c>
+      <c r="G47" s="61" t="n">
         <v/>
       </c>
-      <c r="B36" s="170" t="n"/>
-      <c r="C36" s="170" t="n"/>
-      <c r="D36" s="188" t="n"/>
-      <c r="E36" s="85" t="n"/>
-      <c r="F36" s="191" t="n"/>
-      <c r="G36" s="188" t="n"/>
-      <c r="H36" s="191" t="n"/>
-      <c r="I36" s="188" t="n"/>
-    </row>
-    <row r="37" ht="60" customFormat="1" customHeight="1" s="6" thickBot="1">
-      <c r="A37" s="191" t="n"/>
-      <c r="B37" s="170" t="n"/>
-      <c r="C37" s="170" t="n"/>
-      <c r="D37" s="188" t="n"/>
-      <c r="E37" s="85" t="n"/>
-      <c r="F37" s="191" t="n"/>
-      <c r="G37" s="188" t="n"/>
-      <c r="H37" s="191" t="n"/>
-      <c r="I37" s="188" t="n"/>
-    </row>
-    <row r="38" ht="60" customFormat="1" customHeight="1" s="6" thickBot="1">
-      <c r="A38" s="191" t="n"/>
-      <c r="B38" s="170" t="n"/>
-      <c r="C38" s="170" t="n"/>
-      <c r="D38" s="188" t="n"/>
-      <c r="E38" s="85" t="n"/>
-      <c r="F38" s="191" t="n"/>
-      <c r="G38" s="188" t="n"/>
-      <c r="H38" s="191" t="n"/>
-      <c r="I38" s="188" t="n"/>
-    </row>
-    <row r="39" ht="60" customFormat="1" customHeight="1" s="6" thickBot="1">
-      <c r="A39" s="191" t="n"/>
-      <c r="B39" s="170" t="n"/>
-      <c r="C39" s="170" t="n"/>
-      <c r="D39" s="188" t="n"/>
-      <c r="E39" s="85" t="n"/>
-      <c r="F39" s="191" t="n"/>
-      <c r="G39" s="188" t="n"/>
-      <c r="H39" s="191" t="n"/>
-      <c r="I39" s="188" t="n"/>
-    </row>
-    <row r="40" ht="60" customFormat="1" customHeight="1" s="6" thickBot="1">
-      <c r="A40" s="191" t="n"/>
-      <c r="B40" s="170" t="n"/>
-      <c r="C40" s="170" t="n"/>
-      <c r="D40" s="188" t="n"/>
-      <c r="E40" s="85" t="n"/>
-      <c r="F40" s="191" t="n"/>
-      <c r="G40" s="188" t="n"/>
-      <c r="H40" s="191" t="n"/>
-      <c r="I40" s="188" t="n"/>
-    </row>
-    <row r="41" ht="60" customFormat="1" customHeight="1" s="6" thickBot="1">
-      <c r="A41" s="191" t="n"/>
-      <c r="B41" s="170" t="n"/>
-      <c r="C41" s="170" t="n"/>
-      <c r="D41" s="188" t="n"/>
-      <c r="E41" s="85" t="n"/>
-      <c r="F41" s="191" t="n"/>
-      <c r="G41" s="188" t="n"/>
-      <c r="H41" s="191" t="n"/>
-      <c r="I41" s="188" t="n"/>
-    </row>
-    <row r="42" ht="60" customFormat="1" customHeight="1" s="6" thickBot="1">
-      <c r="A42" s="191" t="n"/>
-      <c r="B42" s="170" t="n"/>
-      <c r="C42" s="170" t="n"/>
-      <c r="D42" s="188" t="n"/>
-      <c r="E42" s="85" t="n"/>
-      <c r="F42" s="191" t="n"/>
-      <c r="G42" s="188" t="n"/>
-      <c r="H42" s="191" t="n"/>
-      <c r="I42" s="188" t="n"/>
-    </row>
-    <row r="43" ht="60" customFormat="1" customHeight="1" s="6" thickBot="1">
-      <c r="A43" s="191" t="n"/>
-      <c r="B43" s="170" t="n"/>
-      <c r="C43" s="170" t="n"/>
-      <c r="D43" s="188" t="n"/>
-      <c r="E43" s="85" t="n"/>
-      <c r="F43" s="191" t="n"/>
-      <c r="G43" s="188" t="n"/>
-      <c r="H43" s="191" t="n"/>
-      <c r="I43" s="188" t="n"/>
-    </row>
-    <row r="44" ht="60" customFormat="1" customHeight="1" s="6" thickBot="1">
-      <c r="A44" s="191" t="n"/>
-      <c r="B44" s="170" t="n"/>
-      <c r="C44" s="170" t="n"/>
-      <c r="D44" s="188" t="n"/>
-      <c r="E44" s="85" t="n"/>
-      <c r="F44" s="191" t="n"/>
-      <c r="G44" s="188" t="n"/>
-      <c r="H44" s="191" t="n"/>
-      <c r="I44" s="188" t="n"/>
-    </row>
-    <row r="45" ht="6" customHeight="1" thickBot="1">
-      <c r="A45" s="54" t="n"/>
-      <c r="B45" s="185" t="n"/>
-      <c r="C45" s="185" t="n"/>
-      <c r="D45" s="185" t="n"/>
-      <c r="E45" s="185" t="n"/>
-      <c r="F45" s="185" t="n"/>
-      <c r="G45" s="185" t="n"/>
-      <c r="H45" s="185" t="n"/>
-      <c r="I45" s="184" t="n"/>
-    </row>
-    <row r="46" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A46" s="192" t="inlineStr">
-        <is>
-          <t>4ª ETAPA - EFICÁCIA</t>
-        </is>
-      </c>
-      <c r="B46" s="157" t="n"/>
-      <c r="C46" s="157" t="n"/>
-      <c r="D46" s="157" t="n"/>
-      <c r="E46" s="178" t="n"/>
-      <c r="F46" s="130" t="inlineStr">
-        <is>
-          <t>Data</t>
-        </is>
-      </c>
-      <c r="G46" s="86" t="inlineStr">
-        <is>
-          <t>04/01/2024</t>
-        </is>
-      </c>
-      <c r="H46" s="170" t="n"/>
-      <c r="I46" s="188" t="n"/>
-    </row>
-    <row r="47" ht="18.75" customHeight="1">
-      <c r="A47" s="158" t="n"/>
-      <c r="E47" s="159" t="n"/>
-      <c r="F47" s="134" t="inlineStr">
-        <is>
-          <t>Resp.:</t>
-        </is>
-      </c>
-      <c r="G47" s="80" t="inlineStr">
-        <is>
-          <t>Amanda Prado</t>
-        </is>
-      </c>
-      <c r="H47" s="157" t="n"/>
-      <c r="I47" s="178" t="n"/>
+      <c r="H47" s="168" t="n"/>
+      <c r="I47" s="169" t="n"/>
     </row>
     <row r="48" ht="25.5" customHeight="1">
-      <c r="A48" s="135" t="inlineStr">
+      <c r="A48" s="89" t="inlineStr">
         <is>
           <t>As ações corretivas foram eficazes? (Caso não, abrir nova RNC)</t>
         </is>
       </c>
-      <c r="B48" s="152" t="n"/>
-      <c r="C48" s="152" t="n"/>
-      <c r="D48" s="152" t="n"/>
-      <c r="E48" s="152" t="n"/>
-      <c r="F48" s="152" t="n"/>
-      <c r="G48" s="152" t="n"/>
-      <c r="H48" s="152" t="n"/>
-      <c r="I48" s="153" t="n"/>
+      <c r="B48" s="144" t="n"/>
+      <c r="C48" s="144" t="n"/>
+      <c r="D48" s="144" t="n"/>
+      <c r="E48" s="144" t="n"/>
+      <c r="F48" s="144" t="n"/>
+      <c r="G48" s="144" t="n"/>
+      <c r="H48" s="144" t="n"/>
+      <c r="I48" s="145" t="n"/>
       <c r="J48" s="4" t="n"/>
       <c r="K48" s="4" t="n"/>
       <c r="L48" s="4" t="n"/>
@@ -2933,38 +2997,38 @@
       <c r="AA48" s="4" t="n"/>
     </row>
     <row r="49" ht="25.5" customHeight="1">
-      <c r="A49" s="88" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="B49" s="193" t="n"/>
-      <c r="C49" s="193" t="n"/>
-      <c r="D49" s="193" t="n"/>
-      <c r="E49" s="193" t="n"/>
-      <c r="F49" s="193" t="n"/>
-      <c r="G49" s="194" t="n"/>
-      <c r="H49" s="137" t="inlineStr">
+      <c r="A49" s="78" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="B49" s="186" t="n"/>
+      <c r="C49" s="186" t="n"/>
+      <c r="D49" s="186" t="n"/>
+      <c r="E49" s="186" t="n"/>
+      <c r="F49" s="186" t="n"/>
+      <c r="G49" s="149" t="n"/>
+      <c r="H49" s="87" t="inlineStr">
         <is>
           <t>Nº da RNC:</t>
         </is>
       </c>
-      <c r="I49" s="10" t="n"/>
+      <c r="I49" s="80" t="n"/>
     </row>
     <row r="50" ht="36.75" customHeight="1">
-      <c r="A50" s="138" t="inlineStr">
+      <c r="A50" s="88" t="inlineStr">
         <is>
           <t>INFORMAÇÕES ADICIONAIS</t>
         </is>
       </c>
-      <c r="B50" s="152" t="n"/>
-      <c r="C50" s="152" t="n"/>
-      <c r="D50" s="152" t="n"/>
-      <c r="E50" s="152" t="n"/>
-      <c r="F50" s="152" t="n"/>
-      <c r="G50" s="152" t="n"/>
-      <c r="H50" s="152" t="n"/>
-      <c r="I50" s="153" t="n"/>
+      <c r="B50" s="144" t="n"/>
+      <c r="C50" s="144" t="n"/>
+      <c r="D50" s="144" t="n"/>
+      <c r="E50" s="144" t="n"/>
+      <c r="F50" s="144" t="n"/>
+      <c r="G50" s="144" t="n"/>
+      <c r="H50" s="144" t="n"/>
+      <c r="I50" s="145" t="n"/>
       <c r="J50" s="4" t="n"/>
       <c r="K50" s="4" t="n"/>
       <c r="L50" s="4" t="n"/>
@@ -2985,27 +3049,29 @@
       <c r="AA50" s="4" t="n"/>
     </row>
     <row r="51" ht="42.75" customFormat="1" customHeight="1" s="6">
-      <c r="A51" s="195" t="inlineStr">
-        <is>
-          <t>Manual da Qualidade aprovado pela consultora Andrea Monteiro.</t>
-        </is>
-      </c>
-      <c r="I51" s="159" t="n"/>
+      <c r="A51" s="187" t="n">
+        <v/>
+      </c>
+      <c r="I51" s="185" t="n"/>
     </row>
     <row r="52" ht="42.75" customFormat="1" customHeight="1" s="6" thickBot="1">
-      <c r="A52" s="180" t="n"/>
-      <c r="B52" s="162" t="n"/>
-      <c r="C52" s="162" t="n"/>
-      <c r="D52" s="162" t="n"/>
-      <c r="E52" s="162" t="n"/>
-      <c r="F52" s="162" t="n"/>
-      <c r="G52" s="162" t="n"/>
-      <c r="H52" s="162" t="n"/>
-      <c r="I52" s="163" t="n"/>
+      <c r="A52" s="171" t="n"/>
+      <c r="B52" s="158" t="n"/>
+      <c r="C52" s="158" t="n"/>
+      <c r="D52" s="158" t="n"/>
+      <c r="E52" s="158" t="n"/>
+      <c r="F52" s="158" t="n"/>
+      <c r="G52" s="158" t="n"/>
+      <c r="H52" s="158" t="n"/>
+      <c r="I52" s="159" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="83">
-    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="A43:D43"/>
     <mergeCell ref="A48:I48"/>
     <mergeCell ref="A50:I50"/>
     <mergeCell ref="A51:I52"/>
@@ -3015,28 +3081,19 @@
     <mergeCell ref="A46:E47"/>
     <mergeCell ref="G46:I46"/>
     <mergeCell ref="G47:I47"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="F38:G38"/>
     <mergeCell ref="A39:D39"/>
     <mergeCell ref="F39:G39"/>
     <mergeCell ref="A40:D40"/>
     <mergeCell ref="F40:G40"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A36:D36"/>
     <mergeCell ref="A33:D34"/>
     <mergeCell ref="E33:E34"/>
     <mergeCell ref="F33:G34"/>
     <mergeCell ref="H33:I34"/>
     <mergeCell ref="A35:D35"/>
     <mergeCell ref="F35:G35"/>
+    <mergeCell ref="H35:I35"/>
     <mergeCell ref="B29:I29"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="C30:I30"/>
@@ -3077,7 +3134,6 @@
     <mergeCell ref="B3:F4"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="G4:H4"/>
-    <mergeCell ref="H35:I35"/>
     <mergeCell ref="H36:I36"/>
     <mergeCell ref="H37:I37"/>
     <mergeCell ref="H38:I38"/>
@@ -3088,6 +3144,12 @@
     <mergeCell ref="H42:I42"/>
     <mergeCell ref="H43:I43"/>
     <mergeCell ref="H44:I44"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="F38:G38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>